<commit_message>
Update the example project
</commit_message>
<xml_diff>
--- a/example-banny-sammy/src/Banny-Sammy-metada-translations.xlsx
+++ b/example-banny-sammy/src/Banny-Sammy-metada-translations.xlsx
@@ -1016,13 +1016,15 @@
 CLOUD SAVE easily syncs the game between your devices and unlocks the full game features when connected to the Internet. 
 PLAY WITH FRIENDS with more fun by sending and asking for lives, friend score ranking, watching friends on the map, sharing your best results, and requesting help from friends. 
 UNIVERSAL — Different graphics are set to fit all of your devices. Enjoy the crisp characters on your phones and tablets. 
-Already a fan of Roll and Eat?
+Already a fan of BannySammy?
   - Visit our official site at http://www.senspark.com
   - Send your feedback via feedback@senspark.com
  -- Like &amp; follow on https://www.facebook.com/TeamSenspark</t>
+- Like &amp; follow on https://www.facebook.com/TeamSenspark
+*** Permissions ***
+GET_ACCOUNTS: Only used if you want to log in or play with your friends via Google + or receive push notification</t>
   </si>
   <si>
     <t>Джунглей полна продуктов для наших милых обезьян и медведей, Сэмми и Банни. Одна проблема: Препятствия предотвратить животных от достижения своих любимых лечит. Попробуйте найти путь, который ведет их к бананы и мед банки и многое другое.
@@ -1037,10 +1039,12 @@
 CLOUD SAVE легко синхронизируется игру между вашими устройствами и разблокирует все возможности игры при подключении к Интернету.
 Играть с друзьями с более увлекательным, посылая и просить жизни, друга оценка рейтинга, наблюдая друзей на карте, разделяя свои лучшие результаты, и с просьбой о помощи от друзей.
 УНИВЕРСАЛЬНЫЙ - Различные графики устанавливаются с учетом всех ваших устройств. Наслаждайтесь четкие символы на ваши телефоны и планшеты.
-Уже поклонник ролл и съесть?
+Уже поклонник BannySammy?
 - Посетите наш официальный сайт по адресу http://www.senspark.com
 - Отправьте обратную связь через feedback@senspark.com
-- Как и следовать по https://www.facebook.com/TeamSenspark</t>
+- Как и следовать по https://www.facebook.com/TeamSenspark
+*** Разрешения ***
+GET_ACCOUNTS: используется только, если вы хотите войти в систему или играть с друзьями с помощью Google + или получить толчок уведомление</t>
   </si>
   <si>
     <t>ป่าที่เต็มไปด้วยอาหารสำหรับลิงน่ารักของเราและหมีแซมมี่และ Banny ปัญหาหนึ่ง: อุปสรรคป้องกันสัตว์จากการเข้าถึงถือว่าพวกเขาชื่นชอบ พยายามที่จะหาเส้นทางที่นำพวกเขาไปกล้วยและน้ำผึ้งขวดและอื่น ๆ
@@ -1055,10 +1059,12 @@
 CLOUD ง่ายประหยัดซิงค์เกมระหว่างอุปกรณ์ของคุณและปลดล็อคคุณสมบัติเกมเต็มรูปแบบเมื่อเชื่อมต่อกับอินเทอร์เน็ต
 เล่นกับเพื่อนด้วยความสนุกสนานมากขึ้นโดยการส่งและขอให้ชีวิตของเพื่อนการจัดอันดับคะแนน, ดูเพื่อนบนแผนที่ร่วมกันผลลัพธ์ที่ดีที่สุดของคุณและขอความช่วยเหลือจากเพื่อน ๆ
 UNIVERSAL - กราฟิกที่แตกต่างกันมีการตั้งค่าให้เหมาะสมกับอุปกรณ์ทั้งหมดของคุณ เพลิดเพลินไปกับตัวอักษรที่คมชัดบนโทรศัพท์และแท็บเล็ตของคุณ
-แล้วแฟนของม้วนและกิน?
+แล้วแฟนของ BannySammy หรือไม่?
 - เยี่ยมชมเว็บไซต์อย่างเป็นทางการของเราที่ http://www.senspark.com
 - ส่งความคิดเห็นของคุณผ่านทาง feedback@senspark.com
-- ชอบและติดตามบน https://www.facebook.com/TeamSenspark</t>
+- ชอบและติดตามบน https://www.facebook.com/TeamSenspark
+สิทธิ์ *** ***
+GET_ACCOUNTS: ใช้เฉพาะในกรณีที่คุณต้องการที่จะเข้าสู่ระบบหรือเล่นกับเพื่อน ๆ ของคุณผ่าน Google + หรือรับการแจ้งเตือนผลักดัน</t>
   </si>
   <si>
     <t>orman bizim sevimli maymunlar ve ayılar, Sammy ve Banny gıdalar doludur. Tek sorun: Engeller sevdikleri davranır ulaşmasını hayvanlar önlemek. muz ve bal kavanoz ve daha fazlası götüren yolu bulmaya çalışın.
@@ -1073,10 +1079,12 @@
 CLOUD TASARRUF kolayca cihazlar arasındaki maçı syncs ve Internet'e bağlandığınızda tam oyun özellikleri kilidini açar.
 arkadaşlar yardım göndermek ve yaşamları için soran arkadaş puanı sıralamasında, harita üzerinde arkadaş izlerken, en iyi sonuçları paylaşmak ve talep ederek daha eğlenceli arkadaşlarınızla oynayın.
 UNIVERSAL - Farklı grafikler cihazların tüm uyacak şekilde ayarlanır. senin telefonlarda ve tabletlerde net karakterler keyfini çıkarın.
-Zaten and Roll hayranı yiyin?
+Zaten BannySammy hayranı?
 - Http://www.senspark.com adresindeki resmi sitesini ziyaret edin
 - Feedback@senspark.com üzerinden görüşlerinizi gönderin
-- Gibi &amp; https://www.facebook.com/TeamSenspark takip</t>
+- Gibi &amp; https://www.facebook.com/TeamSenspark takip
+*** İzinler ***
+GET_ACCOUNTS: giriş veya Google + 'yoluyla arkadaşlarınızla oynamak ya da push bildirimi almak istiyorsanız Sadece kullanılan</t>
   </si>
   <si>
     <t>Rừng là đầy đủ các loại thức ăn cho khỉ dễ thương của chúng tôi và gấu, Sammy và Banny. Một vấn đề: Những trở ngại ngăn cản các con vật từ đạt món yêu thích của họ. Hãy cố gắng tìm ra con đường dẫn họ đến chuối và lọ mật ong và nhiều hơn nữa.
@@ -1091,10 +1099,12 @@
 CLOUD LƯU dễ dàng đồng bộ hóa các trò chơi giữa các thiết bị của bạn và mở khóa các tính năng trò chơi đầy đủ khi kết nối với Internet.
 CHƠI VỚI BẠN BÈ với nhiều niềm vui bằng cách gửi và yêu cầu cuộc sống, người bạn số điểm xếp hạng, xem bạn bè trên bản đồ, chia sẻ kết quả tốt nhất của bạn, và yêu cầu giúp đỡ từ bạn bè.
 UNIVERSAL - đồ họa khác nhau được thiết lập để phù hợp với tất cả các thiết bị của bạn. Thưởng thức các nhân vật rõ nét trên điện thoại và máy tính bảng của bạn.
-Đã là fan hâm mộ của Roll và ăn?
+Đã là fan hâm mộ của BannySammy?
 - Truy cập trang web chính thức của chúng tôi tại http://www.senspark.com
 - Gửi thông tin phản hồi của bạn thông qua feedback@senspark.com
-- Giống như &amp; theo trên https://www.facebook.com/TeamSenspark</t>
+- Giống như &amp; theo trên https://www.facebook.com/TeamSenspark
+*** Quyền ***
+GET_ACCOUNTS: Chỉ sử dụng nếu bạn muốn đăng nhập hoặc chơi với bạn bè của bạn thông qua Google + hoặc nhận thông báo push</t>
   </si>
   <si>
     <t>الغابة مليئة الأطعمة لدينا القرود والدببة لطيف، وسامي وباني. مشكلة واحدة: عقبات تمنع الحيوانات من الوصول يعامل المفضلة لديهم. محاولة للعثور على المسار الذي يؤدي بهم إلى الموز والعسل الجرار وأكثر من ذلك.
@@ -1109,10 +1119,12 @@
 CLOUD SAVE المصاحبة بسهولة في المباراة بين الأجهزة الخاصة بك ويفتح ملامح اللعبة الكاملة عند الاتصال بالإنترنت.
 اللعب مع الأصدقاء مع أكثر متعة من خلال إرسال وطلب الأرواح، صديق النتيجة مرتبة، ومشاهدة الأصدقاء على الخريطة، وتبادل أفضل النتائج الخاصة بك، وطلب المساعدة من الأصدقاء.
 UNIVERSAL - يتم تعيين رسومات مختلفة لتناسب جميع الأجهزة الخاصة بك. استمتع الشخصيات واضحة على الهواتف والأجهزة اللوحية.
-إذا كنت من محبي اللف وصالات؟
+إذا كنت من محبي BannySammy؟
 - زيارة الموقع الرسمي لدينا في http://www.senspark.com
 - إرسال ملاحظاتك عبر feedback@senspark.com
-- مثل وتابع على https://www.facebook.com/TeamSenspark</t>
+- مثل وتابع على https://www.facebook.com/TeamSenspark
+*** *** ضوابط
+GET_ACCOUNTS: يستخدم فقط إذا كنت ترغب في تسجيل الدخول أو اللعب مع أصدقائك عبر جوجل + أو تلقي إشعار الدفع</t>
   </si>
   <si>
     <t>La jungle est plein d'aliments pour nos singes et les ours mignon, Sammy et Banny. Un problème: Les obstacles empêchent les animaux d'atteindre leurs friandises préférées. Essayez de trouver le chemin qui les mène aux bananes et pots de miel et plus.
@@ -1127,10 +1139,12 @@
 CLOUD SAUVEGARDER synchronise facilement le jeu entre vos appareils et déverrouille les fonctionnalités de jeu lors de la connexion à Internet.
 Jouer avec des amis avec plus de plaisir en envoyant et en demandant la vie, un ami pointage de classement, en regardant des amis sur la carte, en partageant vos meilleurs résultats, et de demander l'aide d'amis.
 UNIVERSAL - Différents graphiques sont mis à répondre à tous vos appareils. Profitez des personnages croustillants sur vos téléphones et tablettes.
-Déjà fan de Roll et Eat?
+Déjà fan de BannySammy?
 - Visitez notre site officiel à http://www.senspark.com
 - Envoyer vos commentaires via feedback@senspark.com
-- Comme &amp; suivre sur https://www.facebook.com/TeamSenspark</t>
+- Comme &amp; suivre sur https://www.facebook.com/TeamSenspark
+*** Autorisations ***
+GET_ACCOUNTS: Seulement utilisé si vous voulez vous connecter ou jouer avec vos amis via Google + ou recevoir une notification push</t>
   </si>
   <si>
     <t>Der Dschungel ist voller Lebensmittel für unsere niedlichen Affen und Bären, Sammy und Banny. Ein Problem: Hindernisse, die Tiere daran hindern, ihre Lieblings-Leckereien zu erreichen. Versuchen Sie, den Weg zu finden, um sie zu Bananen und Honiggläser und mehr führt.
@@ -1145,10 +1159,12 @@
 Cloud-Speicher synchronisiert leicht, das Spiel zwischen Ihren Geräten und entriegelt die volle Spiel-Funktionen, wenn mit dem Internet verbunden.
 MIT FREUNDEN mit mehr Spaß spielen, indem sie das Senden und bat um Leben, Freund-Score Ranking, Freunde auf der Karte, teilen Sie Ihre besten Ergebnisse, und anfragende Hilfe von Freunden zu beobachten.
 UNIVERSAL - Verschiedene Grafiken sind so eingestellt, alle Ihre Geräte zu passen. Genießen Sie die gestochen scharfe Zeichen auf Handys und Tabletten.
-Schon ein Fan von Rollen und essen?
+Schon ein Fan von BannySammy?
 - Besuchen Sie unsere offizielle Webseite http://www.senspark.com
 - Senden Sie Ihr Feedback über feedback@senspark.com
-- Like &amp; folgen auf https://www.facebook.com/TeamSenspark</t>
+- Like &amp; folgen auf https://www.facebook.com/TeamSenspark
+*** Berechtigungen ***
+GET_ACCOUNTS: Wird nur verwendet, wenn Sie eingeloggt sein wollen oder mit Ihren Freunden über Google + spielen oder Push-Benachrichtigung erhalten</t>
   </si>
   <si>
     <t>丛林充满食物为我们可爱的猴子和熊，萨米和班尼。问题一：阻碍这些动物到达他们最喜欢的食物。试图找到导致他们的香蕉和蜂蜜罐子和更多的路径。
@@ -1163,10 +1179,12 @@
 云端储存轻松同步你的设备之间的博弈，当连接到互联网解锁完整的游戏功能。
 向朋友们发送和要求的生活，朋友得分排名，看着朋友们在地图上，分享你的最好的结果，并请求帮助一起玩的朋友有更多的乐趣。
 通用 - 不同的图形设置，以适应所有设备。享受你的手机和平板电脑的清脆的字符。
-已经辊和风扇吃？
+已经BannySammy的粉丝吗？
 - 访问我们的官方网站在http://www.senspark.com
 - 通过feedback@senspark.com意见征集
-- 像与遵循https://www.facebook.com/TeamSenspark</t>
+- 像与遵循https://www.facebook.com/TeamSenspark
+*** ***权限
+GET_ACCOUNTS：只有当你想登录或通过谷歌+发挥你的朋友或接收推送通知使用</t>
   </si>
   <si>
     <t>叢林充滿食物為我們可愛的猴子和熊，薩米和班尼。問題一：阻礙這些動物到達他們最喜歡的食物。試圖找到導致他們的香蕉和蜂蜜罐子和更多的路徑。
@@ -1181,10 +1199,12 @@
 雲端儲存輕鬆同步你的設備之間的博弈，當連接到互聯網解鎖完整的遊戲功能。
 向朋友們發送和要求的生活，朋友得分排名，看著朋友們在地圖上，分享你的最好的結果，並請求幫助一起玩的朋友有更多的樂趣。
 通用 - 不同的圖形設置，以適應所有設備。享受你的手機和平板電腦的清脆的字符。
-已經輥和風扇吃？
+已經BannySammy的粉絲嗎？
 - 訪問我們的官方網站在http://www.senspark.com
 - 通過feedback@senspark.com意見徵集
-- 像與遵循https://www.facebook.com/TeamSenspark</t>
+- 像與遵循https://www.facebook.com/TeamSenspark
+*** ***權限
+GET_ACCOUNTS：只有當你想登錄或通過谷歌+發揮你的朋友或接收推送通知使用</t>
   </si>
   <si>
     <t>ジャングルは、私たちのかわいいサルやクマ、サミーとBanny用食品の完全です。一つの問題：障害は自分の好きなお菓子に到達するから動物を防ぎます。バナナと蜂蜜の瓶以上にそれらを導くパスを検索してみてください。
@@ -1199,10 +1219,12 @@
 クラウド保存が簡単にあなたのデバイス間でゲームを同期すると、インターネットに接続したときにフルゲームの特徴のロックを解除します。
 友人からの助けを送信し、生活を求めて、友人をスコアランキング、地図上で友人を見て、あなたの最高の結果を共有し、そして要求することにより、より楽しいと友達と遊びます。
 UNIVERSALは - 異なるグラフィックスがすべてのデバイスに合うように設定されています。あなたの携帯電話やタブレットで鮮明な文字をお楽しみください。
-既にロールのファンと食べますか？
+既にBannySammyのファン？
 - http://www.senspark.comで私たちの公式サイトをご覧ください
 - feedback@senspark.com経由であなたのフィードバックを送信
-- 同様＆https://www.facebook.com/TeamSensparkに従ってください</t>
+- 同様＆https://www.facebook.com/TeamSensparkに従ってください
+***アクセス許可***
+GET_ACCOUNTS：あなたは、ログインするか、Google +を介してお友達と遊ぶか、プッシュ通知を受信したい場合にのみ使用</t>
   </si>
   <si>
     <t>La selva está llena de alimentos para nuestros monos y osos lindo, Sammy y Banny. Uno de los problemas: Los obstáculos impiden que los animales lleguen a sus golosinas favoritas. Tratar de encontrar el camino que les lleva a los plátanos y tarros de miel y mucho más.
@@ -1217,10 +1239,12 @@
 Almacenamiento en la nube se sincroniza fácilmente el juego entre sus dispositivos y desbloquea todas las características del juego cuando está conectado a Internet.
 Juega con tus amigos con más diversión mediante el envío y pidiendo vidas, amigo puntuación de la clasificación, ver amigos en el mapa, para compartir sus mejores resultados, y solicitando la ayuda de amigos.
 UNIVERSAL - se establecen diferentes gráficos para adaptarse a todos los dispositivos. Disfrutar de los caracteres nítidos en sus teléfonos y tabletas.
-Ya es fan de rollo y coma?
+Ya es fan de BannySammy?
 - Visita nuestro sitio oficial en http://www.senspark.com
 - Envía tus comentarios a través de feedback@senspark.com
-- Al igual que en https://www.facebook.com/TeamSenspark y sigue</t>
+- Al igual que en https://www.facebook.com/TeamSenspark y sigue
+*** *** Permisos
+GET_ACCOUNTS: Sólo se utiliza si desea iniciar sesión en o jugar con tus amigos a través de Google + o recibir notificación de inserción</t>
   </si>
   <si>
     <t>La giungla è pieno di alimenti per le nostre scimmie carino e orsi, Sammy e Banny. Un problema: Ostacoli impediscono agli animali di raggiungere i loro preferito tratta. Prova a trovare il percorso che li porta a banane e barattoli di miele e molto altro ancora.
@@ -1235,10 +1259,12 @@
 CLOUD SAVE sincronizza con facilità il gioco tra i dispositivi e sblocca le funzionalità complete del gioco quando si è connessi a Internet.
 Gioca con gli amici con più divertimento con l'invio di e chiedendo per la vita, amico punteggio classifica, a guardare gli amici sulla mappa, condividere i vostri risultati migliori, e la richiesta di aiuto da amici.
 UNIVERSALE - grafica diversa sono impostati per soddisfare tutti i vostri dispositivi. Godetevi i caratteri nitidi sui vostri cellulari e tablet.
-Già un fan di rotolo e mangia oggi?
+Già un fan di BannySammy?
 - Visita il nostro sito ufficiale all'indirizzo http://www.senspark.com
 - Invia i tuoi commenti via feedback@senspark.com
-- Come e segui su https://www.facebook.com/TeamSenspark</t>
+- Come e segui su https://www.facebook.com/TeamSenspark
+*** *** Permessi
+GET_ACCOUNTS: usata solo se si desidera effettuare il login o giocare con i tuoi amici tramite Google + o ricevere notifiche push</t>
   </si>
   <si>
     <t>De jungle is vol met voedsel voor onze leuke apen en beren, Sammy en Banny. Eén probleem: Obstakels te voorkomen dat de dieren uit het bereiken van hun favoriete lekkernijen. Probeer het pad dat leidt naar bananen en honing potten en nog veel meer.
@@ -1253,10 +1279,12 @@
 CLOUD SAVE gemakkelijk synchroniseert de wedstrijd tussen uw apparaten en ontsluit de volledige game features wanneer aangesloten op het internet.
 Spelen met vrienden met meer plezier door het sturen en vragen om het leven, vriend score ranking, het kijken naar vrienden op de kaart, het delen van uw beste resultaten, en het aanvragen van hulp van vrienden.
 UNIVERSAL - Verschillende graphics zijn ingesteld op al uw apparaten te passen. Geniet van de heldere tekens op uw telefoons en tablets.
-Al een fan van Roll en eten?
+Al een fan van BannySammy?
 - Bezoek onze officiële plaats bij http://www.senspark.com
 - Stuur uw terugkoppeling via feedback@senspark.com
-- Net &amp; volg op https://www.facebook.com/TeamSenspark</t>
+- Net &amp; volg op https://www.facebook.com/TeamSenspark
+*** Machtigingen ***
+GET_ACCOUNTS: Wordt alleen gebruikt als je wilt om in te loggen of speel met je vrienden via Google + of ontvangen push notificatie</t>
   </si>
   <si>
     <t>정글은 우리의 귀여운 원숭이와 곰, 새미와 Banny을위한 음식이 가득합니다. 하나의 문제 : 장애물이 자신이 좋아하는 간식에 도달 동물을 방지 할 수 있습니다. 바나나와 꿀 항아리 더로 이어지는 경로를 찾아보십시오.
@@ -1271,10 +1299,12 @@
 클라우드 저장 쉽게 장치 사이에 게임을 동기화하고 인터넷에 연결되어있을 때 전체 게임 기능을 잠금 해제합니다.
 친구의 도움을주고 삶을 요청, 친구 점수 순위,지도에서 친구를보고, 최선의 결과를 공유하고, 요청하여 더 많은 재미와 함께 친구와 함께 플레이.
 UNIVERSAL은 - 다른 그래픽은 모든 장치에 맞게 설정되어 있습니다. 귀하의 휴대 전화와 태블릿에 선명 문자를 즐길 수 있습니다.
-이미와 롤의 팬 먹어?
+이미 BannySammy의 팬?
 - http://www.senspark.com에 우리의 공식 웹 사이트를 방문하십시오
 - feedback@senspark.com 통해 의견 보내기
-- 추천 및 https://www.facebook.com/TeamSenspark에 따라</t>
+- 추천 및 https://www.facebook.com/TeamSenspark에 따라
+*** 권한 ***
+GET_ACCOUNTS : 당신이 로그인하거나 구글 +를 통해 친구와 함께 재생하거나 푸시 알림을 수신 할 경우에만 사용</t>
   </si>
   <si>
     <t>A selva é cheia de alimentos para os nossos macacos e ursos bonitos, Sammy e Banny. Um problema: Obstáculos evitar que os animais de alcançar seus deleites favoritos. Tente encontrar o caminho que os leva a bananas e potes de mel e muito mais.
@@ -1289,10 +1319,12 @@
 CLOUD SALVAR sincroniza facilmente o jogo entre seus dispositivos e desbloqueia as características do jogo completo quando conectado à Internet.
 Jogar com os amigos com mais diversão enviando e pedindo vidas, amigo pontuação no ranking, observando amigos no mapa, compartilhando seus melhores resultados, e solicitando a ajuda de amigos.
 UNIVERSAL - gráficos diferentes estão definidas para caber todos os seus dispositivos. Aproveite os personagens nítidas em seus telefones e tablets.
-Já é um fã de Roll e comer?
+Já é um fã de BannySammy?
 - Visite o nosso site oficial em http://www.senspark.com
 - Feedback via feedback@senspark.com
-- Como &amp; siga em https://www.facebook.com/TeamSenspark</t>
+- Como &amp; siga em https://www.facebook.com/TeamSenspark
+*** *** Permissão
+GET_ACCOUNTS: utilizado somente se você quiser fazer login ou jogar com seus amigos através do Google + ou receber notificações push</t>
   </si>
   <si>
     <t>Viidakko on täynnä elintarvikkeita meidän söpö apinoilla ja karhuja, Sammy ja Banny. Yksi ongelma: Esteet estetään eläinten saavuttamasta suosikki kohtelee. Yritä löytää polku, joka johtaa heidät banaaneja ja hunajan tölkit ja enemmän.
@@ -1307,10 +1339,12 @@
 Pilvitallennus- helposti synkronoi pelin välillä laitteiden ja avaa koko pelin ominaisuuksia, kun yhteys Internetiin.
 Pelaa ystävien kanssa hauskempaa lähettämällä ja pyytävät elämää, ystävä pisteet ranking, katsellen ystäviä kartalla, jaat parhaat tulokset, ja pyytävät apua ystäviltä.
 UNIVERSAL - Eri grafiikka asetetaan sopivat kaikki laitteet. Nauti rapeaksi merkkejä puhelimet ja tabletit.
-Jo fani Roll ja syödä?
+Jo fani BannySammy?
 - Käy virallisella sivustolla osoitteessa http://www.senspark.com
 - Lähetä palautetta kautta feedback@senspark.com
-- Like &amp; seurata https://www.facebook.com/TeamSenspark</t>
+- Like &amp; seurata https://www.facebook.com/TeamSenspark
+*** Oikeudet ***
+GET_ACCOUNTS: Käytetään vain, jos haluat kirjautua sisään tai pelata ystävien kautta Google + tai vastaanottaa push ilmoituksen</t>
   </si>
   <si>
     <t>Jungelen er full av mat til våre søte apekatter og bjørner, Sammy og Banny. Ett problem: Hindringer hindre dyrene fra å nå deres favoritt godbiter. Prøv å finne stien som fører dem til bananer og honning krukker og mer.
@@ -1325,10 +1359,12 @@
 CLOUD LAGRE synkroniserer lett spillet mellom enhetene og låser hele spillet funksjoner når den er koblet til Internett.
 Spill med venner med mer moro ved å sende og ber om liv, venn poengsum rangering, se venner på kartet, dele dine beste resultater, og ber om hjelp fra venner.
 UNIVERSAL - Ulike grafikk er satt til å passe alle enhetene dine. Nyt skarpe tegn på telefoner og nettbrett.
-Allerede en fan av Roll og spise?
+Allerede en fan av BannySammy?
 - Besøk vår offisielle hjemmeside på http://www.senspark.com
 - Send tilbakemelding via feedback@senspark.com
-- Like &amp; følge på https://www.facebook.com/TeamSenspark</t>
+- Like &amp; følge på https://www.facebook.com/TeamSenspark
+*** tillatelser ***
+GET_ACCOUNTS: brukes kun hvis du ønsker å logge inn eller leke med vennene dine via Google + eller motta push-varsling</t>
   </si>
   <si>
     <t>Junglen er fuld af fødevarer til vores søde aber og bjørne, Sammy og Banny. Et problem: Forhindringer forhindre dyrene i at nå deres foretrukne godbidder. Prøv at finde den vej, der fører dem til bananer og honning krukker og meget mere.
@@ -1343,10 +1379,12 @@
 CLOUD SAVE nemt synkroniserer spillet mellem dine enheder og låser det fulde spil funktioner, når forbundet til internettet.
 Spil med venner med mere sjov ved at sende og beder om liv, ven score ranking, ser venner på kortet, dele dine bedste resultater, og anmoder om hjælp fra venner.
 UNIVERSAL - Forskellige grafik er sat til at passe alle dine enheder. Nyd de sprøde tegn på dine telefoner og tabletter.
-Allerede en fan af Roll og spise?
+Allerede en fan af BannySammy?
 - Besøg vores officielle hjemmeside på http://www.senspark.com
 - Send din tilbagemelding via feedback@senspark.com
-- Ligesom &amp; følg på https://www.facebook.com/TeamSenspark</t>
+- Ligesom &amp; følg på https://www.facebook.com/TeamSenspark
+*** Tilladelser ***
+GET_ACCOUNTS: Kun bruges, hvis du ønsker at logge på eller lege med dine venner via Google + eller modtage push-meddelelse</t>
   </si>
   <si>
     <t>Djungeln är full av livsmedel för våra söta apor och björnar, Sammy och Banny. Ett problem: Hinder hindra djuren från att nå sina favoritgodsaker. Försök att hitta den väg som leder dem till bananer och honung burkar och mer.
@@ -1359,12 +1397,14 @@
 Fantastisk grafik och ljud - Känn grafiska detaljer och väl blandade ljud. Det finns fyra olika miljöer och alla är så livlig med dag- och natt bakgrunder, vädereffekter, och massor av animationer. Tecknen "gullighet är outhärdlig.
 SPELA SPEL SERVICE lämnar höga poäng och låser upp massor av framgångar för roligare.
 Molnlagring synkroniserar lätt spelet mellan enheterna och låser hela spelet funktioner när den är ansluten till Internet.
-Spela med vänner med roligare genom att sända och ber om liv, vän poäng rankning, titta vänner på kartan, att dela dina bästa resultat, och begär hjälp från vänner.
+Spela med vänner med roligare genom att sända och be om lives, vän värdering rankning, titta vänner på kartan, att dela dina bästa resultat, och begär hjälp från vänner.
 UNIVERSAL - Olika grafik är inställda för att passa alla dina enheter. Njut av skarpa tecken på dina telefoner och surfplattor.
-Redan ett fan av Roll och äta?
+Redan ett fan av BannySammy?
 - Besök vår officiella hemsida på http://www.senspark.com
 - Skicka feedback via feedback@senspark.com
-- Som och följ på https://www.facebook.com/TeamSenspark</t>
+- Som och följ på https://www.facebook.com/TeamSenspark
+*** Behörigheter ***
+GET_ACCOUNTS: Används endast om du vill logga in eller spela med dina vänner via Google + eller ta emot push-anmälan</t>
   </si>
   <si>
     <t>Dżungla jest pełna żywności dla naszych słodkie małpy i niedźwiedzie, Sammy i Banny. Jeden problem: Przeszkody uniemożliwić zwierzętom dotarcie swoje ulubione smakołyki. Spróbuj znaleźć ścieżkę, która prowadzi ich do bananów i słoików miodu i wiele innych.
@@ -1379,16 +1419,18 @@
 CLOUD SAVE łatwo synchronizuje się mecz pomiędzy urządzeniami i odkrywa pełnię możliwości gry po podłączeniu do Internetu.
 Grać z przyjaciółmi z więcej zabawy poprzez wysyłanie i prosząc o życiu, przyjacielu wynik rankingu, obserwując znajomych na mapie, dzieląc swoje najlepsze rezultaty, i prosząc o pomoc przyjaciół.
 UNIVERSAL - Różne grafiki znajdują się zmieścić wszystkich urządzeń. Ciesz się wyraźnych znaków na telefonach i tabletach.
-Już fanem Roll and Eat?
+Już fanem BannySammy?
 - Odwiedź oficjalną stronę na http://www.senspark.com
 - Wyślij swoją opinię poprzez feedback@senspark.com
-- Podobnie jak i śledź na https://www.facebook.com/TeamSenspark</t>
+- Podobnie jak i śledź na https://www.facebook.com/TeamSenspark
+*** *** Uprawnienia
+GET_ACCOUNTS: używany tylko jeśli chcesz zalogować się lub bawić się z przyjaciółmi za pośrednictwem Google + lub odbierać powiadomienia push</t>
   </si>
   <si>
     <t>Džungle je plná potravin pro naše roztomilé opice a medvědi, Sammy a Banny. Jeden problém: Překážky brání zvířatům dosažení jejich oblíbené pochoutky. Pokuste se najít cestu, která je vede k banány a med sklenic a další.
 *** Hru ***
 Pomáhat zvířatům vrátit do jejich potravy. Opice jíst banány, jablka, hrušky a, a medvědi jíst lososa a med. Dřevěné bloky jsou dělitelné, zatímco kamenné bloky nejsou. Existuje více herní položky přijít s instrukcemi ve hře v průběhu hry.
-*** Herní prvky ***
+*** Hry funkce ***
 4 epizody s 144 rovinách - K dispozici je 36 úrovní v každém ročním období: jaro, podzim, zima a léto. Každý z nich má různé položky hry a tedy i jinou strategii pro krmení opice a medvědi.
 Jedinečný herní s mozek škádlení FUN - interakci s prostředím na pomoc zvířatům vrátit. Obtížnost se zvyšuje v průběhu hry. Dokonce i když se hladina již vymazán, můžete se vrátit později k získání 3-hvězdičkové odznaky. Také budete chtít pokusit se dokončit hru co nejrychleji získat nejvyšší skóre.
 Power-ups jsou užitečné vypořádat s náročnými úrovněmi.
@@ -1397,10 +1439,12 @@
 CLOUD SAVE snadno synchronizuje hru mezi vašimi zařízeními a odemkne plnou hru funkce při připojení k Internetu.
 Zahrajte si s přáteli s více zábavy zasláním a žádají o život, příteli skóre pořadí, sledování přátele na mapě, sdílet své nejlepší výsledky, a požádat o pomoc od přátel.
 UNIVERSAL - různé grafiky jsou nastaveny, aby se vešly ve všech svých zařízeních. Vychutnejte si ostrý znaky na své telefony a tablety.
-Již fanoušek Roll a jíst?
+Již fanoušek BannySammy?
 - Navštivte naše oficiální webové stránky na http://www.senspark.com
 - Odeslat svůj názor prostřednictvím feedback@senspark.com
-- Jako &amp; sledovat na https://www.facebook.com/TeamSenspark</t>
+- Jako &amp; sledovat na https://www.facebook.com/TeamSenspark
+*** Oprávnění ***
+GET_ACCOUNTS: Používá se pouze v případě, že chcete přihlásit, nebo hrát se svými přáteli prostřednictvím služby Google + nebo přijímat push notifikaci</t>
   </si>
   <si>
     <t>Η ζούγκλα είναι γεμάτη τρόφιμα για χαριτωμένο πιθήκους και τις αρκούδες μας, Sammy και Banny. Ένα πρόβλημα: Εμπόδια εμποδίζει τα ζώα από το να επιτύχουν το αγαπημένο τους μεταχειρίζεται. Προσπαθήστε να βρείτε το δρόμο που τους οδηγεί σε μπανάνες και βάζα μέλι και άλλα.
@@ -1415,10 +1459,12 @@
 CLOUD SAVE συγχρονίζει εύκολα το παιχνίδι μεταξύ των συσκευών σας και ξεκλειδώνει τα πλήρη χαρακτηριστικά παιχνίδι, όταν είναι συνδεδεμένος στο Internet.
 Παίξτε με τους φίλους με πιο διασκεδαστικό με την αποστολή και ζητώντας τη ζωή, ο φίλος βαθμολογία κατάταξης, βλέποντας τους φίλους στο χάρτη, την ανταλλαγή βέλτιστων αποτελεσμάτων σας, και ζητώντας βοήθεια από τους φίλους.
 UNIVERSAL - Διαφορετικές γραφικών που να χωρέσει όλες τις συσκευές σας. Απολαύστε τις ευκρινείς χαρακτήρες σε τηλέφωνα και τα δισκία σας.
-Ήδη ένας ανεμιστήρας των Roll και να φάτε;
+Ήδη ένας ανεμιστήρας του BannySammy;
 - Επισκεφτείτε την επίσημη ιστοσελίδα μας στο http://www.senspark.com
 - Στείλτε τα σχόλιά σας μέσω feedback@senspark.com
-- Όπως και ακολουθούν σε https://www.facebook.com/TeamSenspark</t>
+- Όπως και ακολουθούν σε https://www.facebook.com/TeamSenspark
+*** Δικαιώματα ***
+GET_ACCOUNTS: Χρησιμοποιείται μόνο αν θέλετε να συνδεθείτε ή να παίξετε με τους φίλους σας μέσω του Google + ή να λαμβάνετε ειδοποίηση push</t>
   </si>
   <si>
     <t>Джунглів сповнена продуктів для наших милих мавп і ведмедів, Семмі і Банні. Одна проблема: Перешкоди запобігти тварин від досягнення своїх улюблених лікує. Спробуйте знайти шлях, який веде їх до банани і мед банки і багато іншого.
@@ -1433,10 +1479,12 @@
 CLOUD SAVE легко синхронізується гру між вашими пристроями та розблокує всі можливості гри при підключенні до Інтернету.
 Грати з друзями з більш захоплюючим, посилаючи і просити життя, друга оцінка рейтингу, спостерігаючи друзів на карті, розділяючи свої кращі результати, і з проханням про допомогу від друзів.
 УНІВЕРСАЛЬНИЙ - Різні графіки встановлюються з урахуванням всіх ваших пристроїв. Насолоджуйтесь чіткі символи на ваші телефони та планшети.
-Уже шанувальник рол і з'їсти?
+Уже шанувальник BannySammy?
 - Відвідайте наш офіційний сайт за адресою http://www.senspark.com
 - Надішліть зворотний зв'язок через feedback@senspark.com
-- Як і слідувати по https://www.facebook.com/TeamSenspark</t>
+- Як і слідувати по https://www.facebook.com/TeamSenspark
+*** Дозволи ***
+GET_ACCOUNTS: використовується тільки, якщо ви хочете увійти в систему або грати з друзями за допомогою Google + або отримати поштовх повідомлення</t>
   </si>
   <si>
     <t>hutan ini penuh dengan makanan untuk monyet comel dan beruang, Sammy dan Banny. Satu masalah: Halangan menghalang haiwan daripada sampai merawat kegemaran mereka. Cuba untuk mencari jalan yang membawa mereka untuk pisang dan balang madu dan banyak lagi.
@@ -1451,10 +1499,12 @@
 CLOUD JIMAT mudah mensegerakkan permainan antara peranti anda dan membuka ciri-ciri permainan penuh apabila disambungkan ke Internet.
 BERMAIN DENGAN KAWAN dengan lebih seronok dengan menghantar dan meminta nyawa, rakan skor kedudukan, menonton rakan-rakan di peta, berkongsi hasil terbaik anda, dan meminta bantuan daripada rakan-rakan.
 UNIVERSAL - Grafik yang berbeza ditetapkan untuk memenuhi semua peranti anda. Nikmati aksara segar pada telefon dan tablet anda.
-Sudah peminat Roll dan Makan?
+Sudah peminat BannySammy?
 - Lawati laman rasmi kami di http://www.senspark.com
 - Hantar maklum balas anda melalui feedback@senspark.com
-- Like &amp; ikuti di https://www.facebook.com/TeamSenspark</t>
+- Like &amp; ikuti di https://www.facebook.com/TeamSenspark
+*** *** Kebenaran
+GET_ACCOUNTS: Hanya digunakan jika anda mahu log masuk atau bermain dengan kawan-kawan anda melalui Google + atau menerima pemberitahuan menolak</t>
   </si>
   <si>
     <t>hutan ini penuh dengan makanan untuk monyet lucu dan beruang, Sammy dan Banny. Satu masalah: Hambatan mencegah hewan dari mencapai memperlakukan favorit mereka. Cobalah untuk menemukan jalan yang mengarah ke pisang dan guci madu dan banyak lagi.
@@ -1469,10 +1519,12 @@
 CLOUD HEMAT mudah sync pertandingan antara perangkat Anda dan membuka fitur permainan lengkap ketika terhubung ke Internet.
 BERMAIN DENGAN TEMAN dengan lebih menyenangkan dengan mengirimkan dan meminta kehidupan, teman skor peringkat, menonton teman-teman di peta, berbagi hasil terbaik Anda, dan meminta bantuan dari teman.
 UNIVERSAL - grafis yang berbeda ditetapkan untuk cocok untuk semua perangkat Anda. Nikmati karakter renyah di ponsel Anda dan tablet.
-Sudah penggemar Roll dan Makan?
+Sudah penggemar BannySammy?
 - Kunjungi situs resmi kami di http://www.senspark.com
 - Kirim masukan Anda melalui feedback@senspark.com
-- Seperti &amp; ikuti di https://www.facebook.com/TeamSenspark</t>
+- Seperti &amp; ikuti di https://www.facebook.com/TeamSenspark
+*** Izin ***
+GET_ACCOUNTS: Hanya digunakan jika Anda ingin login atau bermain dengan teman-teman Anda melalui Google + atau menerima pemberitahuan push</t>
   </si>
   <si>
     <t>Jungla este plin de alimente pentru maimuțe noastre drăguț și urși, Sammy și Banny. O problema: obstacolele care împiedică animalele să ajungă la tratează lor preferate. Încercați să găsiți calea pe care le conduce la banane și borcane de miere și multe altele.
@@ -1487,10 +1539,12 @@
 CLOUD SAVE sincronizeaza cu ușurință jocul dintre dispozitivele și deblochează caracteristicile complete de joc atunci când este conectat la Internet.
 Joace cu prietenii cu mai multă distracție prin trimiterea și cerând viață, prieten scor clasament, vizionarea prieteni pe hartă, schimbul de cele mai bune rezultate, și solicitarea de ajutor de la prieteni.
 UNIVERSAL - Diferite grafice sunt setate pentru a se potrivi toate dispozitivele. Bucurați-vă de caractere clare pe telefoane și tablete.
-Deja un fan al roll și mânca?
+Deja un fan al BannySammy?
 - Vizitati site-ul nostru oficial de la http://www.senspark.com
 - Trimite feedback-ul prin feedback@senspark.com
-- La fel ca și urmați pe https://www.facebook.com/TeamSenspark</t>
+- La fel ca și urmați pe https://www.facebook.com/TeamSenspark
+*** Permisiuni ***
+GET_ACCOUNTS: utilizați numai dacă doriți să conectați sau să se joace cu prietenii prin intermediul Google + sau de a primi notificare push</t>
   </si>
   <si>
     <t>הג'ונגל הוא מלא של מזונות עבור הקופים החמודים שלנו ודובים, סמי Banny. בעיה אחת: מכשולי למנוע החיות מלהגיע הפינוקים האהובים עליהם. נסה למצוא את הנתיב שמוביל אותם בננות וצנצנות דבש ועוד.
@@ -1505,10 +1559,12 @@
 שמירה בענן בקלות מסנכרנת את המשחק בין המכשירים שלך ואת פותחת את התכונות מלאות משחק כאשר מחוברת לאינטרנט.
 לשחק עם חברים עם יותר כיף על ידי שליחת ומבקש חייהם, חבר ציון הדירוג, צופה החברים על המפה, שיתוף התוצאות הטובות ביותר שלך, ולבקש עזרה מחברים.
 UNIVERSAL - גרפיקה שונה נקבע כדי להתאים את כל המכשירים שלך. תהין הדמויות הפריכות בטלפונים וטאבלטים שלך.
-כבר אוהד של רול לאכול?
+כבר אוהד של BannySammy?
 - בקרו באתר הרשמי שלנו בכתובת http://www.senspark.com
 - שלח את המשוב שלך באמצעות feedback@senspark.com
-- כמו ומעקב אחר על https://www.facebook.com/TeamSenspark</t>
+- כמו ומעקב אחר על https://www.facebook.com/TeamSenspark
+*** הרשאות ***
+GET_ACCOUNTS: השתמש רק אם אתה רוצה להיכנס או לשחק עם החברים שלך דרך גוגל + או כדי לקבל הודעת דחיפה</t>
   </si>
   <si>
     <t>जंगल हमारे प्यारा बंदरों और भालू, सैमी और Banny के लिए खाद्य पदार्थ से भरा हुआ है। एक समस्या यह है: बाधाओं को उनके पसंदीदा व्यवहार पहुंचने से जानवरों को रोकने के। रास्ता है कि उन्हें केले और शहद के जार और अधिक करने के लिए सुराग खोजने की कोशिश करें।
@@ -1523,10 +1579,12 @@
 बादल सहेजें आसानी से अपने उपकरणों के बीच खेल सिंक करता है और जब इंटरनेट से जुड़ा पूरा खेल सुविधाओं बातें बताता है।
 दोस्तों से दोस्त की मदद भेजने और जीवन के लिए पूछ रही है, स्कोर रैंकिंग, नक्शे पर दोस्तों को देख, अपने सबसे अच्छा परिणाम साझा करने, और अनुरोध द्वारा अधिक मज़ा के साथ दोस्तों के साथ खेलने।
 यूनिवर्सल - अलग ग्राफिक्स अपने सभी उपकरणों को फिट करने के लिए सेट कर रहे हैं। अपने फोन और टैबलेट पर कुरकुरा पात्रों का आनंद लें।
-पहले से ही रोल और एक प्रशंसक खाओ?
+पहले से ही BannySammy के एक प्रशंसक?
 - Http://www.senspark.com पर हमारे आधिकारिक साइट पर जाएँ
 - Feedback@senspark.com के माध्यम से अपनी प्रतिक्रिया भेजें
-- जैसा और https://www.facebook.com/TeamSenspark पर का पालन करें</t>
+- जैसा और https://www.facebook.com/TeamSenspark पर का पालन करें
+*** *** अनुमतियां
+GET_ACCOUNTS: ही इस्तेमाल करता है, तो आप में प्रवेश करें या गूगल + के माध्यम से अपने दोस्तों के साथ खेलने के लिए या धक्का अधिसूचना प्राप्त करना चाहते हैं</t>
   </si>
   <si>
     <t>Джунгляў поўная прадуктаў для нашых мілых малпаў і мядзведзяў, Сэмі і Бані. Адна праблема: Перашкоды прадухіліць жывёл ад дасягнення сваіх любімых лечыць. Паспрабуйце знайсці шлях, які вядзе іх да бананы і мёд банкі і многае іншае.
@@ -1541,10 +1599,12 @@
 CLOUD SAVE лёгка сінхранізуецца гульню паміж вашымі прыладамі і разблакуе ўсе магчымасці гульні пры падключэнні да Інтэрнэту.
 Гуляць з сябрамі з больш займальным, пасылаючы і прасіць жыцця, сябра адзнака рэйтынгу, назіраючы сяброў на карце, падзяляючы свае лепшыя вынікі, і з просьбай аб дапамозе ад сяброў.
 Універсальнасць - Розныя графікі ўсталёўваюцца з улікам усіх вашых прылад. Атрымлівайце асалоду ад выразныя сімвалы на вашыя тэлефоны і планшэты.
-Ужо прыхільнік рол і з'есці?
+Ужо прыхільнік BannySammy?
 - Наведайце наш афіцыйны сайт па адрасе http://www.senspark.com
 - Адпраўце зваротную сувязь праз feedback@senspark.com
-- Як і рухацца па https://www.facebook.com/TeamSenspark</t>
+- Як і рухацца па https://www.facebook.com/TeamSenspark
+*** Дазволу ***
+GET_ACCOUNTS: выкарыстоўваецца толькі, калі вы хочаце ўвайсці ў сістэму або гуляць з сябрамі з дапамогай Google + або атрымаць штуршок апавяшчэнне</t>
   </si>
   <si>
     <t>Джунглата е пълна с храни за нашите сладки маймуни и мечки, Сами и Banny. Един проблем: Препятствия пречат на животните от достигането на любимите си лакомства. Опитайте се да намерите пътя, който ги кара да банани и мед буркани и повече.
@@ -1559,10 +1619,12 @@
 Запазване в облака лесно се синхронизира играта между устройствата си и отключва пълните функции на играта, когато е свързан към интернет.
 Играе с приятели с по-забавно, като изпрати и молба за живота, приятел на полувремето класиране, гледане на приятелите си на картата, споделяне на най-добрите си резултати, и с молба за помощ от приятели.
 UNIVERSAL - Различни графики са настроени да се поберат всички ваши устройства. Насладете се на отчетливи героите на вашите телефони и таблети.
-Още един фен на Roll и яде?
+Още един фен на BannySammy?
 - Посетете нашия официален сайт на http://www.senspark.com
 - Изпращане на обратна информация чрез feedback@senspark.com
-- Както и да следва по https://www.facebook.com/TeamSenspark</t>
+- Както и да следва по https://www.facebook.com/TeamSenspark
+*** Разрешения ***
+GET_ACCOUNTS: Само използват, ако желаете да се регистрирате или да играе с приятелите си чрез Google + или получавате известие за предаване</t>
   </si>
   <si>
     <t>gubat ay puno ng mga pagkain para sa aming mga cute na monkeys at bear, Sammy at Banny. Isang problema: Obstacles maiwasan ang mga hayop mula sa maabot ang kanilang mga paboritong GFPFE. Subukan upang mahanap ang landas na patungo sa kanila na saging at honey garapon at higit pa.
@@ -1577,10 +1639,12 @@
 CLOUD SAVE madaling syncs ang laro sa pagitan ng iyong device at magbubukas ang buong mga tampok ng laro kapag nakakonekta sa Internet.
 MAGLARO SA MGA KAIBIGAN na may mas masaya sa pamamagitan ng pagpapadala at humihingi ng buhay, kaibigan marka ranggo, nanonood mga kaibigan sa mapa, pagbabahagi ng iyong pinakamahusay na mga resulta, at humihiling ng tulong mula sa mga kaibigan.
 UNIVERSAL - Iba't ibang graphics ay nakatakda upang magkasya ang lahat ng iyong device. Damhin ang matalim na mga character sa iyong phone at tablet.
-Mayroon isang fan ng Roll at Kumain?
+Mayroon isang fan ng BannySammy?
 - Bisitahin ang aming opisyal na site sa http://www.senspark.com
 - Ipadala ang iyong puna sa pamamagitan ng feedback@senspark.com
-- Like &amp; sundin sa https://www.facebook.com/TeamSenspark</t>
+- Like &amp; sundin sa https://www.facebook.com/TeamSenspark
+*** Pahintulot ***
+GET_ACCOUNTS: Tanging gamitin kung gusto mong mag-log in o makipaglaro sa iyong mga kaibigan sa pamamagitan ng Google + o makatanggap ng push notification</t>
   </si>
   <si>
     <t>Džungla je pun hrane za naše slatka majmuna i medvjeda, Sammy i Banny. Jedan od problema: Prepreke spriječiti životinje da dođe do svoje omiljene poslastice. Pokušajte pronaći put koji ih vodi do banana i med staklenke i još mnogo toga.
@@ -1595,13 +1659,15 @@
 Spremanje u oblak lako sinkronizira igre između uređaja i otključava pune značajke igre kada je spojen na Internet.
 Igrati se s prijateljima s više zabave slanjem i molba za život, prijatelju rezultat rang, gledajući prijatelje na karti, dijeleći svoje najbolje rezultate, i traži pomoć od prijatelja.
 UNIVERSAL - Različite grafike su postavljeni kako bi odgovarao svim vašim uređajima. Uživajte u jasne znakove o svojim telefone i tablete.
-Već fan Roll i jesti?
+Već ljubitelj BannySammy?
 - Posjetite našu službenu stranicu na http://www.senspark.com
 - Pošaljite povratne informacije putem feedback@senspark.com
-- Kao i pratiti na https://www.facebook.com/TeamSenspark</t>
-  </si>
-  <si>
-    <t>A dzsungel tele élelmiszerek számára aranyos majmok és medvék, Sammy és Banny. Az egyik probléma: akadályok megakadályozzák az állatok elérik kedvenc kezeli. Próbáld megtalálni az utat, amely ahhoz vezet, hogy a banán és üveg mézet és így tovább.
+- Kao i pratiti na https://www.facebook.com/TeamSenspark
+*** Dozvole ***
+GET_ACCOUNTS: Koristi se samo ako želite prijaviti ili igrati sa svojim prijateljima preko Google + ili primiti automatsku obavijest</t>
+  </si>
+  <si>
+    <t>A dzsungel tele élelmiszerek számára aranyos majmok és medvék, Sammy és Banny. Az egyik probléma: akadályok állnak az állatok eljussanak a kedvenc kezeli. Próbáld megtalálni az utat, amely ahhoz vezet, hogy a banán és üveg mézet és így tovább.
 *** *** Vad játék
 Segítség az állatok tekercs, hogy az élelmiszer. Majmok enni banánt, almát, és körtét és medvék enni lazac és a méz. Fahasábokat törhető míg kőtömbök nem. Több játékelemek jönni, in-game utasításokat a játék előrehaladtával.
 *** Játékban ***
@@ -1613,10 +1679,12 @@
 CLOUD SAVE könnyen szinkronizálja a játék között, az eszközök és feloldja a teljes játékban, amikor csatlakozik az internethez.
 Játszani a barátaival, több móka, a küldő és kérnek életük, barát pontszám rangsor, figyelte barátai a térképen, megosztja a legjobb eredményt, és kér segítséget barátok.
 UNIVERSAL - Különböző grafikák vannak beállítva, hogy illeszkedjen az összes eszközt. Élvezze a jól körvonalazott karakterek a telefonok és tablettát.
-Már egy rajongó Roll és enni?
+Már egy rajongó BannySammy?
 - Látogassa meg a hivatalos site-on http://www.senspark.com
 - Küldj visszajelzést keresztül feedback@senspark.com
-- Mint &amp; követik https://www.facebook.com/TeamSenspark</t>
+- Mint &amp; követik https://www.facebook.com/TeamSenspark
+*** *** Engedélyek
+GET_ACCOUNTS: Csak akkor használatos, ha azt szeretné, hogy jelentkezzen be, vagy játszani a barátaival a Google + vagy fogadni push értesítési</t>
   </si>
   <si>
     <t>Džungļi ir pilns ar pārtikas produktiem mūsu gudrs pērtiķiem un lāči, Sammy un Banny. Viena problēma: šķēršļi novērstu dzīvnieku sasniegt savus iecienītākos gardumus. Mēģiniet atrast ceļu, kas ved viņus uz banāniem un medus burkas un vairāk.
@@ -1631,10 +1699,12 @@
 CLOUD SAVE viegli sinhronizē spēli starp jūsu ierīcēm un atslēdz pilna spēle iezīmes, kad izveidots savienojums ar internetu.
 Spēlē ar draugiem ar vairāk jautrības, nosūtot un prasot dzīvi, draugs rezultāts ranking, skatoties draugu kartē, daloties savus labākos rezultātus, un lūdzot palīdzību no draugiem.
 UNIVERSAL - Dažādas grafikas ir noteikti, lai atbilstu visām jūsu ierīcēm. Izbaudiet kraukšķīgus rakstzīmes jūsu tālruņiem un tabletēm.
-Jau ventilators Roll un ēst?
+Jau ventilators BannySammy?
 - Apmeklējiet mūsu oficiālo vietni http://www.senspark.com
 - Nosūtīt atsauksmes via feedback@senspark.com
-- Tāpat kā un seko https://www.facebook.com/TeamSenspark</t>
+- Tāpat kā un seko https://www.facebook.com/TeamSenspark
+*** atļaujas ***
+GET_ACCOUNTS: Tikai izmantot, ja jūs vēlaties, lai pieteiktos vai spēlēt ar saviem draugiem, izmantojot Google + vai saņemt push paziņojumu</t>
   </si>
   <si>
     <t>Џунгла је пуна хране за наше слатке мајмуна и медведа, Самми и Банни. Један проблем: Препреке спречавају животиње да стигну до својих омиљених посластице. Покушајте да пронађете пут који их води до банане и меда тегле и више.
@@ -1649,10 +1719,12 @@
 Цлоуд САВЕ лако синхронизује игру између уређаја и откључава погодности игре када је повезан на Интернет.
 Играње са пријатељима са више забаве слањем и тражећи живот, пријатељу резултат рангирања, гледајући пријатеље на мапи, дељење своје најбоље резултате, и тражи помоћ од пријатеља.
 Универсал - Различити графика су постављени да одговарају свим вашим уређајима. Уживајте у јасне знакове на телефонима и таблетима.
-Већ фан Ролл и Еат?
+Већ фан БанниСамми?
 - Посетите официјални сајт у хттп://ввв.сенспарк.цом
 - Пошаљите повратне информације преко феедбацк@сенспарк.цом
-- Као и пратити на хттпс://ввв.фацебоок.цом/ТеамСенспарк</t>
+- Као и пратити на хттпс://ввв.фацебоок.цом/ТеамСенспарк
+*** Дозволе ***
+ГЕТ_АЦЦОУНТС: користи само уколико желите да се пријавите или се играју са својим пријатељима преко Гоогле + или примити пусх нотификације</t>
   </si>
   <si>
     <t>Džungľa je plná potravín pre naše roztomilé opice a medvede, Sammy a Banny. Jeden problém: Prekážky bránia zvieratám dosiahnutiu ich obľúbené pochúťky. Pokúste sa nájsť cestu, ktorá ich vedie k banány a med pohárov a ďalšie.
@@ -1667,10 +1739,12 @@
 CLOUD SAVE ľahko synchronizuje hru medzi vašimi zariadeniami a odomkne plnú hru funkcie pri pripojení na internet.
 Zahrajte si s priateľmi s viac zábavy zaslaním a žiadajú o život, priateľovi skóre poradí, sledovanie priateľov na mape, zdieľať svoje najlepšie výsledky, a požiadať o pomoc od priateľov.
 UNIVERSAL - rôzne grafiky sú nastavené, aby sa zmestili vo všetkých svojich zariadeniach. Vychutnajte si ostrý znaky na svoje telefóny a tablety.
-Už fanúšik Roll a jesť?
+Už fanúšik BannySammy?
 - Navštívte naše oficiálne webové stránky na http://www.senspark.com
 - Pošli svoj názor prostredníctvom feedback@senspark.com
-- Ako &amp; sledovať na https://www.facebook.com/TeamSenspark</t>
+- Ako &amp; sledovať na https://www.facebook.com/TeamSenspark
+*** Oprávnenie ***
+GET_ACCOUNTS: Používa sa iba v prípade, že chcete prihlásiť, alebo hrať so svojimi priateľmi prostredníctvom služby Google + alebo prijímať push notifikáciu</t>
   </si>
   <si>
     <t>Džungla je poln hrane za naše luštna opicah in medvedi, Sammyja in Banny. En problem: Ovire preprečujejo živali doseže svoje najljubše dobrote. Poskusi, da bi našli pot, ki jih vodi za banane in medu, kozarci in še več.
@@ -1680,15 +1754,17 @@
 4 epizode s 144 RAVNI - Obstaja 36 stopenj v vsaki sezoni: pomlad, jesen, zima in poletje. Vsak od njih ima različne elemente igre in s tem drugačno strategijo za hranjenje opice in medvede.
 Unique igranja z BRAIN-dražila FUN - Interakcija z okoljem za pomoč živalim roll. Težava povečuje kot igra napreduje. Tudi takrat, ko se raven že očiščeno, se lahko vrnete kasneje zaslužil 3 zvezdicami značke. Prav tako boste želeli, da bi poskušali končati igro kakor hitro je mogoče, da bi dobili najvišje ocene.
 POWER-UPS so koristni za reševanje zahtevnih ravneh.
-Super grafika in zvok - Feel grafične podrobnosti in dobro meša zvoke. Obstajajo štiri različne okoljih in vsi so tako živahno z dnevnimi in nočnimi okolij, vremenskimi vplivi in ton animacij. Ljupkost junakov je neznosno.
+Super grafika in zvok - Feel grafične podrobnosti in dobro meša zvoke. Obstajajo štiri različne okoljih in vsi so tako živahno z dnevno in nočno okolij, vremenskimi vplivi in ton animacij. Ljupkost junakov je neznosno.
 PLAY GAME SERVIS navaja visoke ocene in odklene ton dosežke za več zabave.
 CLOUD SAVE enostavno sinhronizira igro med vašimi napravami in odklene vseh funkcij v igro, ko je priključen na internet.
 Igranje s prijatelji z več zabave s pošiljanjem in prosi za življenje, prijatelj ocena razvrstitev, gledal prijatelje na zemljevidu, delijo svoje najboljše rezultate, in zahteva pomoč od prijateljev.
 UNIVERZALNI - Različne grafike so določeni, da ustrezajo vse vaše naprave. Uživajte jasne znake na svojih telefonih in tabličnih računalnikih.
-Že ljubitelj roll in jesti?
+Že oboževalec BannySammy?
 - Obiščite našo uradno stran na http://www.senspark.com
 - Pošljite povratne informacije preko feedback@senspark.com
-- Like in sledite https://www.facebook.com/TeamSenspark</t>
+- Like in sledite https://www.facebook.com/TeamSenspark
+*** Dovoljenja ***
+GET_ACCOUNTS: uporabljajo samo, če želite, da se prijavite ali igrajo s prijatelji prek storitve Google + ali prejeti obvestilo, naročeno</t>
   </si>
   <si>
     <t>Die woud is vol kos vir ons oulike ape en bere, Sammy en Banny. Een probleem: Hindernisse verhoed dat die diere van die bereik van hul gunsteling lekkernye. Probeer om die pad wat hulle lei tot piesangs en heuning potte en meer uit te vind.
@@ -1703,10 +1779,12 @@
 Wolkstoor maklik synchronisaties die wedstryd tussen jou toestelle en ontsluit die volle wedstryd funksies wanneer verbind tot die Internet.
 Speel met vriende met meer pret deur die stuur en vra vir lewe, vriend telling posisie, kyk vriende op die kaart, die deel van jou beste resultate, en vra die hulp van vriende.
 UNIVERSAL - Verskillende beelde is gereed om al jou toestelle te pas. Geniet die helder karakters op jou selfone en tablette.
-Reeds 'n fan van Roll en eet?
+Reeds 'n fan van BannySammy?
 - Besoek ons amptelike webwerf by http://www.senspark.com
 - Stuur jou terugvoer via feedback@senspark.com
-- Soos &amp; volg op https://www.facebook.com/TeamSenspark</t>
+- Soos &amp; volg op https://www.facebook.com/TeamSenspark
+*** Permissions ***
+GET_ACCOUNTS: Slegs gebruik as jy wil om aan te meld of speel met jou vriende via Google + of ontvang stoot kennisgewing</t>
   </si>
   <si>
     <t>ጫካ የእኛን እነኚያ ደስ ጦጣዎች እና ድቦች, Sammy እና Banny ለ ምግቦች የተሞላ ነው. አንድ ችግር: እንቅፋቶችን የሚወዷቸውን ይገመግማል, ለመድረስ ከ እንስሳት ለመከላከል. ሙዝ እና ማር ብልቃጦች እና ተጨማሪ እነሱን በሚወስደው መንገድ ለማግኘት ይሞክሩ.
@@ -1721,10 +1799,12 @@
 የደመና ማስቀመጥ በቀላሉ የእርስዎ መሣሪያዎች መካከል ጨዋታ የሚመሳሰልና ከበይነመረቡ ጋር በሚገናኝበት ጊዜ ሙሉ የጨዋታ ባህሪያት ይከፈታል.
 ከጓደኞች እርዳታ ለመላክ እና ሕይወት በመጠየቅ, ጓደኛ ነጥብ ደረጃ አመዳደብ, በካርታው ላይ ከጓደኞች በመመልከት, ምርጥ ውጤቶች ማጋራት, እና በመጠየቅ ይበልጥ አዝናኝ ጋር ከጓደኞቼ ጋር ለመጫወት.
 ዩኒቨርሳል - የተለያዩ ግራፊክስ በሁሉም መሣሪያዎችዎ ለማስማማት ተዋቅረዋል. በእርስዎ ስልኮች እና ጡባዊዎች ላይ ያለውን ጥርት ቁምፊዎች ይደሰቱ.
-አስቀድሞ ኤንድ ሮል አንድ አድናቂ ብሉ?
+ቀድሞውኑ BannySammy አንድ አድናቂ?
 - Http://www.senspark.com ላይ ያለንን ኦፊሴላዊ ጣቢያ ይጎብኙ
 - Feedback@senspark.com በኩል ግብረ-መልስ ላክ
-- እንደ &amp; https://www.facebook.com/TeamSenspark ላይ ይከተሉ</t>
+- እንደ &amp; https://www.facebook.com/TeamSenspark ላይ ይከተሉ
+*** ፍቃዶች ***
+GET_ACCOUNTS: በእናንተ ውስጥ መግባት ወይም በ Google + በኩል ከጓደኞችህ ጋር መጫወት ወይም የግፋ ማሳወቂያ መቀበል የማይፈልጉ ከሆነ ብቻ ጥቅም ላይ</t>
   </si>
   <si>
     <t>The Jungle լի է սննդի մեր cute Կապիկներ եւ արջերի, Sammy եւ Banny: Մեկ խնդիրը: Խոչընդոտները կանխել կենդանիներին ից հասնելով իրենց սիրած վերաբերվում. Փորձեք գտնել այն ուղին, որը տանում է նրանց բանան ու մեղր բանկա եւ ավելին:
@@ -1739,10 +1819,12 @@
 CLOUD խնայել հեշտ syncs խաղը միջեւ ձեր սարքերի եւ unlocks լրիվ խաղը առանձնահատկություններ, երբ միացված է ինտերնետին:
 Խաղալ ընկերների հետ ավելի զվարճալի ուղարկելով եւ խնդրելով կյանքում, ընկեր հաշիվը դասակարգման, դիտելով ընկերների քարտեզի վրա, կիսելով ձեր լավագույն արդյունքները, եւ պահանջելով, ընկերների օգնության.
 UNIVERSAL - Տարբեր գրաֆիկա սահմանվել են տեղավորել ձեր բոլոր սարքերի. Վայելեք գանգուր սիմվոլները ձեր հեռախոսների եւ Ցուցանակներ.
-Արդեն մի երկրպագու Roll եւ Eat.
+Արդեն մի երկրպագու BannySammy.
 - Այցելեք մեր պաշտոնական կայքը http://www.senspark.com
 - ՈՒղարկել Ձեր կարծիքը միջոցով feedback@senspark.com
-- Like &amp; հետեւել է https://www.facebook.com/TeamSenspark</t>
+- Like &amp; հետեւել է https://www.facebook.com/TeamSenspark
+*** թույլտվություններ ***
+GET_ACCOUNTS: Միայն օգտագործվում է, եթե դուք ուզում եք մուտք գործել, կամ խաղալ ձեր ընկերների միջոցով Google + - կամ ստանալ հրում ծանուցում</t>
   </si>
   <si>
     <t>Jungle bizim cute monkeys və ayı, Sammy və banny üçün ərzaq doludur. Bir problem: Maneələr onların sevimli alır nail heyvanların qarşısını alır. banan və bal bankalar və daha çox onları çıxarır yolu tapmaq üçün cəhd edin.
@@ -1757,10 +1839,12 @@
 CLOUD SAVE asanlıqla cihazlar arasında oyun syncs və Internet bağlı zaman tam oyun xüsusiyyətləri unlocks.
 dostlar yardım göndərilməsi və həyatları üçün xahiş, dost hesab sıralama xəritədə dost seyr, ən yaxşı nəticələri bölüşmək, və tələb daha çox əyləncə ilə dostları ilə oynayır.
 UNIVERSAL - Müxtəlif qrafik cihazlar bütün uyğun müəyyən edilir. Sizin telefon və tablet xırtıldayan simvol malikdirlər.
-Artıq və Roll bir fan yemək?
+Artıq BannySammy bir fan?
 - Http://www.senspark.com bizim rəsmi saytına müraciət edin
 - Feedback@senspark.com vasitəsilə Əlaqə göndər
-- Like &amp; https://www.facebook.com/TeamSenspark edin</t>
+- Like &amp; https://www.facebook.com/TeamSenspark edin
+*** Permissions ***
+GET_ACCOUNTS: daxil olmaq və ya Google + vasitəsilə dostları ilə oynamaq və ya push bildiriş almaq istəyirsinizsə yalnız istifadə</t>
   </si>
   <si>
     <t>oihanean gure tximinoak cute eta hartzak, Sammy eta Banny elikagai betea. Arazoa: Oztopoak animaliak saihesteko bere gogoko tratatzen heltzea. Saiatu doan bidea horiek bananak eta ezti poteak eta gehiago aurkitzeko.
@@ -1775,10 +1859,12 @@
 CLOUD SAVE erraz zure gailu arteko jokoa sinkronizatzen eta joko osoa ezaugarri desblokeatzeko denean Internetera konektatuta.
 Lagunekin jolastu fun gehiago laguntza lagunen laguna bidaliz eta bizitza eskatuz, puntuazio ranking, mapan lagun behaketa, zure emaitzarik onenak partekatzen, eta eskatuz.
 UNIVERSAL - grafiko desberdinak ezarri dira gailu guztietan egokitzeko. Gozatu crisp pertsonaiak zure telefono eta pilulak.
-Dagoeneko Roll eta fan bat jan?
+Dagoeneko BannySammy zalea?
 - Gure gune ofiziala bisitatu http://www.senspark.com at
 - Eusko Jaurlaritza feedback@senspark.com bidez
-- Like &amp; jarraitu on https://www.facebook.com/TeamSenspark</t>
+- Like &amp; jarraitu on https://www.facebook.com/TeamSenspark
+*** *** Baimenak
+GET_ACCOUNTS: bakarrik erabiltzen den saio hasi edo zure lagunekin jolastu Google + bidez zein push jakinarazpen jaso nahi baduzu</t>
   </si>
   <si>
     <t>জঙ্গল আমাদের চতুর বানর, ভালুক, স্যামি ও Banny জন্য খাবার পরিপূর্ণ. একটা সমস্যা: অবমুক্ত তাদের প্রিয় একইরূপে পৌঁছনো থেকে পশুদের প্রতিরোধ. পাথ যে তাদের কলা ও মধু বয়াম এবং আরও বাড়ে খুঁজে পেতে চেষ্টা করুন.
@@ -1793,10 +1879,12 @@
 মেঘ সংরক্ষণ সহজে আপনার ডিভাইসের মধ্যে খেলা সিঙ্ক এবং যখন ইন্টারনেটের সাথে সংযুক্ত পূর্ণ খেলা বৈশিষ্ট্য আনলক হয়ে যাবে.
 বন্ধুদের কাছ থেকে বন্ধু সাহায্যের প্রেরণ এবং জীবনের জন্য জিজ্ঞাসা, স্কোর র্যাংকিং, মানচিত্রে বন্ধুদের পর্যবেক্ষক, আপনার ভাল ফলাফলের ভাগ, এবং অনুরোধ করে আরো মজা সঙ্গে বন্ধুদের সঙ্গে খেলা.
 সর্বজনীন - বিভিন্ন গ্রাফিক্স আপনার সমস্ত ডিভাইসের মাপসই নির্ধারণ করা হয়. আপনার ফোন এবং ট্যাবলেট উপর খাস্তা অক্ষর উপভোগ করুন.
-ইতিমধ্যে রোল এবং একটি ফ্যান খাও?
+ইতিমধ্যে BannySammy একজন অনুরাগী?
 - Http://www.senspark.com এ আমাদের অফিসিয়াল সাইট দেখুন
 - Feedback@senspark.com মাধ্যমে আপনার প্রতিক্রিয়া পাঠান
-- ভালো লেগেছে &amp; https://www.facebook.com/TeamSenspark উপর অনুসরণ</t>
+- ভালো লেগেছে &amp; https://www.facebook.com/TeamSenspark উপর অনুসরণ
+*** অনুমতিসমূহ ***
+GET_ACCOUNTS: ব্যবহৃত যদি আপনি লগ-ইন বা গুগল + এর মাধ্যমে আপনার বন্ধুদের সঙ্গে খেলা বা ধাক্কা বিজ্ঞপ্তি পেতে চাই</t>
   </si>
   <si>
     <t>အဆိုပါတောတွင်းကျွန်တော်တို့ရဲ့ချစ်စရာမျောက်နှင့်ဝံ, Sammy နှင့် Banny များအတွက်အစားအစာနှင့်ပြည့်ဝ၏။ တစျခုမှာပြဿနာ: အခက်အခဲများကိုသူတို့အကြိုက်ဆုံးရယူထားသောရောက်ရှိမှတိရစ္ဆာန်ကာကွယ်တားဆီး။ ငှက်ပျောသီးနှင့်ပျားရည်အိုးနှင့်ပိုပြီးသူတို့ကိုပို့ဆောင်သောလမ်းကိုရှာတွေ့ဖို့ကြိုးစားပါ။
@@ -1811,10 +1899,12 @@
 မိုဃ်းတိမ်ကိုစီး SAVE ကိုအလွယ်တကူသင့်ရဲ့ device များအကြားဂိမ်းအမြဲတမ်းလိုလို sync နှင့်အင်တာနက်ချိတ်ဆက်သည့်အခါအပြည့်အဝဂိမ်း features တွေကိုသော့ဖွင့်။
 မိတျဆှေ, ရာထူးမြေပုံပေါ်တွင်မိတ်ဆွေများကိုကြည့်, သင့်ကိုအကောင်းဆုံးရလဒ်တွေကိုမျှဝေ, အဆွေခင်ပွန်းထံမှအကူအညီတောင်းခံဂိုးသွင်း, ပေးပို့ခြင်းနှင့်ဘဝအဘို့ကိုတောင်းပိုပြီးပျော်စရာနှင့်အတူသူငယ်ချင်းတွေနဲ့အတူ PLAY ။
 ဝဠာ - ကွဲပြားခြားနားတဲ့ဂရပ်ဖစ်သင့်ကိရိယာများအားလုံး fit မှသတ်မှတ်ထားကြသည်။ သင့်ရဲ့ဖုန်းများနှင့် tablet များပေါ်တွင်ကြည်လင်ပြတ်သားတဲ့ဇာတ်ကောင်ခံစားပါ။
-ယခုပင်လျှင်တစ် Roll ၏ပန်ကာများနှင့်စားပါ?
+BannySammy ၏ယခုပင်လျှင်ပရိတ်သတ်?
 - http://www.senspark.com မှာကျွန်တော်တို့ရဲ့အရာရှိတဦး site ကိုသွားရောက်
 - feedback@senspark.com မှတဆင့်သင့်ရဲ့တုံ့ပြန်ချက် Send
-- လိုပဲ &amp; https://www.facebook.com/TeamSenspark အပေါ်နောက်သို့လိုက်</t>
+- လိုပဲ &amp; https://www.facebook.com/TeamSenspark အပေါ်နောက်သို့လိုက်
+*** ခွင့်ပြုချက်များ ***
+GET_ACCOUNTS: သင်လော့ဂ်သို့မဟုတ် Google + ကနေတဆင့်သင့်ရဲ့သူငယ်ချင်းတွေနဲ့အတူကစားသို့မဟုတ်တွန်းအားပေးအကြောင်းကြားစာလက်ခံရရှိရန်လိုလျှင်သာအသုံးပြု</t>
   </si>
   <si>
     <t>La selva és plena d'aliments per als nostres micos i óssos valent, Sammy i Banny. Un dels problemes: Els obstacles impedeixen que els animals arribin als seus llaminadures preferides. Tractar de trobar el camí que els porta als plàtans i pots de mel i molt més.
@@ -1829,10 +1919,12 @@
 Emmagatzematge en el núvol se sincronitza fàcilment el joc entre els seus dispositius i desbloqueja totes les característiques del joc quan està connectat a Internet.
 Juga amb els teus amics amb més diversió mitjançant l'enviament i demanant vides, amic puntuació de la classificació, veure amics al mapa, per compartir els seus millors resultats, i sol·licitant l'ajuda d'amics.
 UNIVERSAL - s'estableixen diferents gràfics per adaptar-se a tots els dispositius. Gaudir dels caràcters nítids en els seus telèfons i tauletes.
-Ja és fan de rotllo i coma?
+Ja és fan de BannySammy?
 - Visita el nostre lloc oficial en http://www.senspark.com
 - Envia els teus comentaris a través de feedback@senspark.com
-- Igual que en https://www.facebook.com/TeamSenspark i segueix</t>
+- Igual que en https://www.facebook.com/TeamSenspark i segueix
+*** *** Permisos
+GET_ACCOUNTS: Només s'utilitza si voleu iniciar sessió en o jugar amb els teus amics a través de Google+ o rebre notificació d'inserció</t>
   </si>
   <si>
     <t>Džungel on täis toitu meie armas ahvid ja karud, Sammy ja Banny. Üks probleem: Takistused vältida loomade jõudmist oma lemmik kohtleb. Püüa leida tee, mis viib neid banaane ja meepotti ja rohkem.
@@ -1847,10 +1939,12 @@
 CLOUD SAVE lihtsalt sünkroniseerib mängu vahele seadmeid ja lukust See mäng kui see on ühendatud internetti.
 Mängi sõpradega koos lõbusam saates ja küsib elu, sõber skoor edetabel, vaadates sõbrad kaardil, jagades oma parimaid tulemusi ning abi paluda sõbrad.
 Universal - Erinevad graafika on sätestatud, et mahutada kõiki oma seadmeid. Naudi karge märki oma telefonid ja tabletid.
-Juba fänn Roll ja süüa?
+Juba fänn BannySammy?
 - Külasta meie ametlik veebileht aadressil http://www.senspark.com
 - Saada oma tagasiside kaudu feedback@senspark.com
-- Nagu &amp; jätkuks https://www.facebook.com/TeamSenspark</t>
+- Nagu &amp; jätkuks https://www.facebook.com/TeamSenspark
+*** Reeglid ***
+GET_ACCOUNTS: Kasutatakse, kui soovite sisse logida või mängida oma sõprade kaudu Google + või saada tõukemärguanne</t>
   </si>
   <si>
     <t>A selva é chea de alimentos para os nosos monos e osos bonitos, Sammy e Banny. Un problema: Obstáculos evitar que os animais de acadar os seus deleites favoritos. Tente atopar o camiño que os leva a bananas e botes de mel e moito máis.
@@ -1865,10 +1959,12 @@
 CLOUD Gardar sincroniza facilmente o xogo entre os seus dispositivos e desbloquea as características do xogo completo cando conectado a Internet.
 Xogar cos amigos con máis diversión enviando e pedindo vidas, amigo puntuación na valoración, observando amigos no mapa, compartindo os seus mellores resultados, e solicitando a axuda de amigos.
 UNIVERSAL - gráficos diferentes están definidas para caber todos os seus dispositivos. Aproveitar os personaxes nítidas nos seus teléfonos e tabletas.
-Xa é un fan de Roll e comer?
+Xa é un fan de BannySammy?
 - Visita a nosa web oficial en http://www.senspark.com
 - Suxestións vía feedback@senspark.com
-- Como &amp; diríxase https://www.facebook.com/TeamSenspark</t>
+- Como &amp; diríxase https://www.facebook.com/TeamSenspark
+*** *** Permiso
+GET_ACCOUNTS: utilizado só se quere facer login ou xogar cos seus amigos a través de Google + ou recibir notificacións push</t>
   </si>
   <si>
     <t>ჯუნგლებში არის სავსე საკვები ჩვენი cute მაიმუნი და დათვი, Sammy და Banny. ერთი პრობლემა: დაბრკოლებები თავიდან ცხოველების მიაღწია მათი საყვარელი ეპყრობა. სცადეთ იპოვოთ გზა, რომელსაც მივყავართ მათ ბანანი და თაფლი ქილებში და სხვა.
@@ -1883,15 +1979,17 @@
 CLOUD SAVE ადვილად სინქრონიზირებს თამაშის შორის თქვენი მოწყობილობების და დართვა სრული თამაში თვისებები, როდესაც ინტერნეტთან.
 ითამაშეთ მეგობრებთან ერთად უფრო სახალისო გაგზავნით და ითხოვს ცხოვრება, მეგობარს ანგარიში რეიტინგში, ყურება მეგობრების რუკაზე, გაზიარება თქვენი საუკეთესო შედეგების, და დახმარებას ითხოვს მეგობრები.
 UNIVERSAL - სხვა და სხვა გრაფიკული უეჭველია, რომ შეესაბამება ყველა თქვენი მოწყობილობების. იხალისეთ crisp გმირები თქვენი ტელეფონები და დაფები.
-უკვე გულშემატკივარი Roll და ჭამა?
+უკვე გულშემატკივარი BannySammy?
 - ეწვიეთ ჩვენს ოფიციალურ საიტზე http://www.senspark.com
 - თქვენი კავშირი მეშვეობით feedback@senspark.com
-- Like და დაიცვას https://www.facebook.com/TeamSenspark</t>
+- Like და დაიცვას https://www.facebook.com/TeamSenspark
+*** ნებართვების ***
+GET_ACCOUNTS: გამოიყენება მხოლოდ იმ შემთხვევაში, თუ გსურთ შესვლა ან ითამაშოთ მეგობრებთან ერთად მეშვეობით Google + ან მიიღოს ბიძგი შეტყობინება</t>
   </si>
   <si>
     <t>Frumskógur er fullur af matvælum fyrir sætu öpum okkar og ber, Sammy og BANNY. Eitt vandamál: Hindranir koma í veg fyrir að dýrin ná uppáhalds skemmtun þeirra. Reyndu að finna leið sem leiðir þá til banana og hunang krukkur og fleira.
 *** Leikur leika ***
-Hjálp dýrin rúlla í fæðu þeirra. Monkeys borða banana, epli og perur, og ber borða lax og hunang. Wood blokkir eru brjóta meðan blokkir steini eru ekki. Það eru fleiri leikur atriði til að koma með í leiknum leiðbeiningar sem leikinn líður.
+Hjálp dýrin rúlla í fæðu þeirra. Monkeys borða banana, epli og perur, og ber borða lax og hunang. Viður blokkir eru brjóta meðan blokkir steini eru ekki. Það eru fleiri leikur atriði til að koma með í leiknum leiðbeiningar sem leikinn líður.
 *** leikur lögun ***
 4 þáttur með 144 stigum - Það eru 36 stig í hvert skipti: Vor, Haust, Vetur, sumar. Hver og einn hefur mismunandi atriði leikur og svona mismunandi stefnu til að fæða öpum og birni.
 Einstaka gameplay með heila-hugsæld gaman - samskipti við umhverfið til að hjálpa dýrin rúlla. Erfiðleikarnir eykst sem leikinn líður. Jafnvel þegar borðin eru nú þegar eytt getur þú komið aftur seinna til að græða 3-stjörnu merkin. Einnig, þú vilt reyna að klára leikinn eins hratt og mögulegt er til að fá hæsta stig.
@@ -1901,10 +1999,12 @@
 CLOUD SAVE samstillir auðveldlega leikinn á milli tæki og kennt fullur leikur lögun þegar það er tengt við internetið.
 Spila með vinum með meiri gaman með því að senda og biðja um líf, vinur skora röðun, horfa vini á kortinu, deila bestu niðurstöður, og biðja hjálp frá vinum.
 UNIVERSAL - Mismunandi grafík ætlar að passa öll tæki. Njóttu skýrar stafi á símum og spjaldtölvum.
-Þegar aðdáandi Roll og borða?
+Þegar aðdáandi BannySammy?
 - Heimsókn opinbera síðuna okkar á http://www.senspark.com
 - Senda álit þitt um feedback@senspark.com
-- Eins og fylgja á https://www.facebook.com/TeamSenspark</t>
+- Eins og fylgja á https://www.facebook.com/TeamSenspark
+*** Heimildir ***
+GET_ACCOUNTS: Aðeins notaðir ef þú vilt skrá þig inn eða spila með vinum þínum í gegnum Google + eða fá ýta tilkynningar</t>
   </si>
   <si>
     <t>ಕಾಡಿನಲ್ಲಿ ನಮ್ಮ ಮುದ್ದಾದ ಕೋತಿಗಳು ಮತ್ತು ಕರಡಿಗಳು, ಸ್ಯಾಮಿ ಮತ್ತು Banny ಆಹಾರಗಳು ತುಂಬಿರುತ್ತವೆ. ಒಂದು ಸಮಸ್ಯೆ: ಅಡೆತಡೆಗಳನ್ನು ಅವರ ನೆಚ್ಚಿನ ಹಿಂಸಿಸಲು ಸಾಗುವುದನ್ನು ಪ್ರಾಣಿಗಳು ತಡೆಗಟ್ಟಲು. ಬಾಳೆಹಣ್ಣುಗಳು ಮತ್ತು ಜೇನು ಜಾಡಿಗಳಲ್ಲಿ ಮತ್ತು ಹೆಚ್ಚು ಅವರನ್ನು ಕಾರಣವಾಗುತ್ತದೆ ಮಾರ್ಗವನ್ನು ಹುಡುಕಲು ಪ್ರಯತ್ನಿಸಿ.
@@ -1919,10 +2019,12 @@
 ಕ್ಲೌಡ್ ಉಳಿಸು ಸುಲಭವಾಗಿ ನಿಮ್ಮ ಸಾಧನಗಳ ನಡುವೆ ಆಟ ಸಿಂಕ್ ಮತ್ತು ಇಂಟರ್ನೆಟ್ ಸಂಪರ್ಕ ಪೂರ್ಣ ಆಟದ ವೈಶಿಷ್ಟ್ಯಗಳನ್ನು ಅನ್ಲಾಕ್.
 ಸ್ನೇಹಿತ ಸ್ನೇಹಿತರಿಂದ, ಸ್ಕೋರ್ ಕಳುಹಿಸುವ ಮತ್ತು ಜೀವನದ ಕೇಳುತ್ತಿದೆ, ಶ್ರೇಯಾಂಕ ನಕ್ಷೆಯಲ್ಲಿ ಸ್ನೇಹಿತರು ವೀಕ್ಷಿಸಲು ನಿಮ್ಮ ಉತ್ತಮ ಫಲಿತಾಂಶಗಳನ್ನು ಹಂಚಿಕೊಳ್ಳಲು, ಮತ್ತು ಮನವಿ ಸಹಾಯ ಮೂಲಕ ಹೆಚ್ಚು ಮೋಜಿನ ಜೊತೆಗೆ ಸ್ನೇಹಿತರೊಂದಿಗೆ ಆಡಲು.
 ಯುನಿವರ್ಸಲ್ - ವಿವಿಧ ಗ್ರಾಫಿಕ್ಸ್ ನಿಮ್ಮ ಸಾಧನಗಳ ಎಲ್ಲಾ ಹೊಂದಿಕೊಳ್ಳಲು ಹೊಂದಿಸಲಾಗಿದೆ. ನಿಮ್ಮ ಫೋನ್ ಮತ್ತು ಟ್ಯಾಬ್ಲೆಟ್ಗಳಲ್ಲಿ ಗರಿಗರಿಯಾದ ಪಾತ್ರಗಳು ಆನಂದಿಸಿ.
-ಈಗಾಗಲೇ ರೋಲ್ ಮತ್ತು ಅಭಿಮಾನಿ ಈಟ್?
+ಈಗಾಗಲೇ BannySammy ಅಭಿಮಾನಿ?
 - Http://www.senspark.com ನಮ್ಮ ಅಧಿಕೃತ ಸೈಟ್ ಭೇಟಿ
 - Feedback@senspark.com ಮೂಲಕ ನಿಮ್ಮ ಪ್ರತಿಕ್ರಿಯೆ ಕಳುಹಿಸಿ
-- ಲೈಕ್ &amp; https://www.facebook.com/TeamSenspark ಮೇಲೆ ಅನುಸರಿಸಿ</t>
+- ಲೈಕ್ &amp; https://www.facebook.com/TeamSenspark ಮೇಲೆ ಅನುಸರಿಸಿ
+*** ಅನುಮತಿಗಳು ***
+GET_ACCOUNTS: ನೀವು ಲಾಗ್ ಇನ್ ಅಥವಾ ಗೂಗಲ್ + ಮೂಲಕ ನಿಮ್ಮ ಸ್ನೇಹಿತರೊಂದಿಗೆ ಆಡಲು ಅಥವಾ ಪುಶ್ ಅಧಿಸೂಚನೆಯನ್ನು ಪಡೆಯಲು ಬಯಸಿದರೆ ಮಾತ್ರ ಬಳಸಲಾಗುತ್ತದೆ</t>
   </si>
   <si>
     <t>ព្រៃនេះគឺជាការពេញលេញនៃអាហារសម្រាប់សត្វស្វានិងខ្លាឃ្មុំគួរឱ្យស្រលាញ់របស់យើង, សាមីនិង Banny ។ បញ្ហាមួយ: ឧបសគ្គរារាំងការសត្វដែលបានមកពីការឈានដល់ការព្យាបាលជំងឺរបស់ពួកគេចូលចិត្ត។ សូមព្យាយាមដើម្បីស្វែងរកផ្លូវដែលនាំពួកគេឱ្យចេកនិងពាងទឹកឃ្មុំនិងច្រើនទៀត។
@@ -1937,10 +2039,12 @@
 cloud រក្សាទុកយ៉ាងងាយស្រួលធ្វើសមកាលកម្មឧបករណ៍របស់អ្នកការប្រកួតរវាងនិងដោះសោលក្ខណៈពិសេសការប្រកួតពេញពេលដែលបានតភ្ជាប់ទៅអ៊ីនធឺណិត។
 លេងជាមួយមិត្តភក្តិជាមួយភាពសប្បាយរីករាយកាន់តែច្រើនដោយការផ្ញើនិងសួរសម្រាប់ជីវិត, មិត្តពិន្ទុចំណាត់ថ្នាក់មើលមិត្តភក្តិនៅលើផែនទី, ការចែករំលែកលទ្ធផលល្អបំផុតរបស់អ្នកនិងស្នើសុំជំនួយពីមិត្តភក្តិ។
 សកល - ក្រាហ្វិកផ្សេងគ្នាត្រូវបានកំណត់ឱ្យសមទៅនឹងឧបករណ៍ទាំងអស់របស់អ្នក។ សូមរីករាយជាមួយតួអក្សរច្បាស់នៅលើទូរស័ព្ទនិង Tablet របស់អ្នក។
-រួចទៅហើយអ្នកគាំទ្ររបស់រមៀលនិងការបរិភោគ?
+រួចទៅហើយជាអ្នកគាំទ្រនៃ BannySammy មួយ?
 - ទស្សនាគេហទំព័រផ្លូវការរបស់យើងនៅ http://www.senspark.com
 - ផ្ញើមតិអ្នកប្រើរបស់អ្នកតាមរយៈ feedback@senspark.com
-- ដូចជាអនុវត្តតាម https://www.facebook.com/TeamSenspark &amp;</t>
+- ដូចជាអនុវត្តតាម https://www.facebook.com/TeamSenspark &amp;
+*** សិទ្ធិ ***
+GET_ACCOUNTS: បានប្រើតែប្រសិនបើអ្នកចង់ចូលលេងជាមួយមិត្តភក្តិរបស់អ្នកតាមរយៈ Google + ឬទទួលបានការជូនដំណឹងការជំរុញ</t>
   </si>
   <si>
     <t>Джунгли Биздин сүйкүмдүү маймылдар жана аюу, Ажар жана Banny үчүн тамак-аш азыктарынын толгон. Бир маселе: тоскоолдуктар, алардын жакшы көргөн мамиле жетүүгө жаныбарларды алдын алуу. банан жана бал кумуралар жана дагы алып барат жолун табууга аракет кылышат.
@@ -1955,10 +2059,12 @@
 Интернетке туташкан кезде CLOUD SAVE оной аппараттардын өз ара оюнду шайкештелет жана толук оюн өзгөчөлүктөрүн кулпусу.
 жөнөтүү жана өмүр сурап көп тамашалуу менен ойноп, досу эсеби даражалуу, картада Досторду карап, жакшы натыйжалары жана достору жардам сурап кайрылган.
 UNIVERSAL - ар түрдүү сүрөттөр Бардык түзмөктөрдөгү ылайык белгиленет. Сиздин уюлдук жана таш лоокторго кытырак белгилерди пайдаланышат.
-Мурда-н-ролл жана бир күйөрман жегиле?
+Буга чейин BannySammy бир күйөрман?
 - Http://www.senspark.com биздин расмий сайтынан
 - Feedback@senspark.com аркылуу пикир жөнөтүү
-- Like &amp; https://www.facebook.com/TeamSenspark боюнча ээрчип</t>
+- Like &amp; https://www.facebook.com/TeamSenspark боюнча ээрчип
+*** Уруксаат ***
+GET_ACCOUNTS: Only Сиз кирүү же Google + аркылуу достору менен ойноп же түртүү билдирүү кабыл алып келсе, колдонулган</t>
   </si>
   <si>
     <t>ໄກ່ປ່າແມ່ນອັນເຕັມທີ່ຂອງອາຫານສໍາລັບ monkeys ງາມຂອງພວກເຮົາແລະຫມີສວນ່, Sammy ແລະ Banny. ຫນຶ່ງໃນບັນຫາ: ອຸປະສັກປ້ອງກັນບໍ່ໃຫ້ສັດຈາກການເຂົ້າເຖິງການປິ່ນປົວ favorite ຂອງເຂົາເຈົ້າ. ພະຍາຍາມເພື່ອຊອກຫາເສັ້ນທາງທີ່ເຮັດໃຫ້ເຂົາເຈົ້າຫມາກກ້ວຍແລະ jars ້ໍາເຜີ້ງແລະອື່ນໆອີກ.
@@ -1973,10 +2079,12 @@
 CLOUD SAVE ໄດ້ຢ່າງງ່າຍດາຍຊິງເກມລະຫວ່າງອຸປະກອນຂອງທ່ານແລະເປີດລັກສະນະເກມອັນເຕັມທີ່ໃນເວລາທີ່ເຊື່ອມຕໍ່ກັບອິນເຕີເນັດ.
 ຫຼິ້ນກັບຫມູ່ເພື່ອນມີຄວາມມ່ວນຫຼາຍໂດຍການສົ່ງແລະການສະເຫນີຂໍສໍາລັບຊີວິດ, ຫມູ່ເພື່ອນຈັດລຽງລໍາດັບ, ການສັງເກດເບິ່ງຫມູ່ເພື່ອນໃນແຜນທີ່, ການແລກປ່ຽນຜົນການຄົ້ນຫາທີ່ດີທີ່ສຸດຂອງທ່ານ, ແລະການຮ້ອງຂໍການຊ່ວຍເຫຼືອຈາກຫມູ່ເພື່ອນ.
 ວິທະຍາໄລ - ຮູບພາບທີ່ແຕກຕ່າງກັນແມ່ນກໍານົດໃຫ້ເຫມາະທັງຫມົດຂອງອຸປະກອນຂອງທ່ານ. ມີຄວາມສຸກລັກສະນະ crisp ກ່ຽວກັບໂທລະສັບມືຖືແລະຢາເມັດຂອງທ່ານ.
-ແລ້ວພັດລົມຂອງມ້ວນແລະກິນອາຫານ?
+ແລ້ວພັດລົມຂອງ BannySammy ເປັນ?
 - ຢ້ຽມຊົມເວັບໄຊຢ່າງເປັນທາງການຂອງພວກເຮົາທີ່ http://www.senspark.com
 - ສົ່ງຄໍາຄຶດຄໍາເຫັນຂອງທ່ານໂດຍຜ່ານ feedback@senspark.com
-- ເຊັ່ນດຽວກັນກັບແລະຕິດຕາມກ່ຽວກັບ https://www.facebook.com/TeamSenspark</t>
+- ເຊັ່ນດຽວກັນກັບແລະຕິດຕາມກ່ຽວກັບ https://www.facebook.com/TeamSenspark
+*** ການອະນຸຍາດ ***
+GET_ACCOUNTS ການນໍາໃຊ້ພຽງແຕ່ຖ້າວ່າທ່ານຕ້ອງການທີ່ຈະເຂົ້າສູ່ລະບົບຫຼືຫຼິ້ນກັບຫມູ່ເພື່ອນຂອງທ່ານໂດຍຜ່ານກູໂກ + ຫລືໄດ້ຮັບແຈ້ງການຊຸກຍູ້</t>
   </si>
   <si>
     <t>Džiunglės yra pilnas maisto produktų mūsų mielas beždžionių ir meškų, Sammy ir Banny. Viena problema: Kliūtys išvengti gyvūnų pasiekti savo mėgstamus skanėstų. Pabandykite surasti kelią, kuris veda juos į bananų ir medaus stiklainius ir daugiau.
@@ -1991,10 +2099,12 @@
 CLOUD Iš SAVE lengvai sinchronizuoja tarp jūsų įrenginius žaidimą ir atrakina visas žaidimo funkcijas, kai prijungtas prie interneto.
 Žaisti su draugais su daugiau įdomus siunčiant ir prašo gyvenime, draugui rezultatas rango, žiūrėti draugus žemėlapyje, dalintis savo geriausius rezultatus, ir prašydama pagalbos iš draugų.
 Universal - Įvairūs Grafika yra nustatyti, kad tilptų visi jūsų įrenginius. Mėgaukitės aiškūs simboliai savo telefonus ir planšetinius kompiuterius.
-Jau roll ir ventiliatorius valgyti?
+Jau yra BannySammy ventiliatorius?
 - Aplankykite mūsų oficialų svetainėje adresu http://www.senspark.com
 - Siųsti atsiliepimą per feedback@senspark.com
-- Kaip ir sekite ant https://www.facebook.com/TeamSenspark</t>
+- Kaip ir sekite ant https://www.facebook.com/TeamSenspark
+*** Leidimai ***
+GET_ACCOUNTS: Tik naudoti, jei norite prisijungti arba žaisti su savo draugais per "Google +" arba gauti pranešimą push</t>
   </si>
   <si>
     <t>Џунглата е полна со храна за нашата симпатична мајмуни, мечки, Семи и Banny. Еден проблем: Пречки спречи животните да стигнат до нивните омилени десерти. Обидете се да најдете на патот кој ги води до банани и мед тегли и многу повеќе.
@@ -2009,10 +2119,12 @@
 CLOUD SAVE лесно се синхронизира играта помеѓу вашите уреди и отклучува сите карактеристики игра кога е поврзан на интернет.
 Игра со пријателите со повеќе забава со испраќање и ја прашува за својот живот, пријател резултат пласман, гледа пријатели на сајтот, споделувањето на вашите најдобри резултати, и бара помош од пријателите.
 УНИВЕРЗАЛНА - Различни графика се поставени за да ги собере сите на вашите уреди. Уживајте во јасни знаци на вашите мобилни телефони и таблети.
-Веќе фан на тек и се јаде?
+Веќе фан на BannySammy?
 - Посетете ја нашата официјална страница на http://www.senspark.com
 - Испрати вашите повратни информации преку feedback@senspark.com
-- Како и следење на https://www.facebook.com/TeamSenspark</t>
+- Како и следење на https://www.facebook.com/TeamSenspark
+*** Дозволи ***
+GET_ACCOUNTS: Се користи само ако сакате да се најавите или да си играат со вашите пријатели преку Google + или примите известување притисок</t>
   </si>
   <si>
     <t>ജംഗിൾ ഞങ്ങളുടെ സൌന്ദര്യമുണ്ട് കുരങ്ങ്, കരടി, സമ്മി എന്നിവ Banny വേണ്ടി ഭക്ഷണങ്ങൾ നിറഞ്ഞിരിക്കുന്നു. ഒരു പ്രശ്നം: തടസ്സങ്ങൾ അവരുടെ പ്രിയപ്പെട്ട ട്രീറ്റുകൾക്കായും ബലിമൃഗങ്ങളെ മൃഗങ്ങളെ തടയാൻ. വാഴപ്പഴം തേനും ജാറുകൾ കൂടുതൽ അവരെ നയിക്കുന്ന പാത കണ്ടെത്താൻ ശ്രമിക്കുക.
@@ -2020,17 +2132,19 @@
 മൃഗങ്ങൾ തങ്ങളുടെ ആഹാരം ഉരുട്ടി സഹായിക്കുക. മങ്കീസ് വാഴ, ആപ്പിൾ, ഒപ്പം pears തിന്നുകയും കരടികളും സാൽമൺ തേനും. കല്ലു ബ്ലോക്കുകൾ ലഭ്യമല്ലെങ്കിലും വുഡ് ബ്ലോക്കുകൾ പൊട്ടാവുന്ന ആകുന്നു. ഗെയിം വർദ്ധിക്കുന്നതിനനുസരിച്ച് പോലെ ഇൻ-ഗെയിം നിർദേശങ്ങൾ കൂടുതൽ ഗെയിം ഇനങ്ങൾ ഉണ്ട്.
 *** ഗെയിം സവിശേഷതകൾ ***
 സ്പ്രിംഗ്, ഓട്ടം, വിന്റർ വേനൽക്കാലത്തു: - 144 തലങ്ങളിൽ 4 എപ്പിസോഡുകൾ ഓരോ സീസണിൽ 36 അളവ് ഉണ്ട്. ഓരോന്നും വ്യത്യസ്ത ഗെയിം ഇനങ്ങൾ അതുവഴി കുരങ്ങുകളും, കരടി ഭക്ഷണം മറ്റൊരു തന്ത്രത്തിന്റെ ഉണ്ട്.
-മസ്തിഷ്ക ബസിലും രസകരമായി സമാനതകളില്ലാത്തതായിരുന്നത് ഗെയിംപ്ലേ - മൃഗങ്ങൾ ഉരുട്ടി സഹായിക്കുന്നതിന് പരിസ്ഥിതി സംവദിക്കുക. ഗെയിം ഗൃഹാതുരന് എന്ന ബുദ്ധിമുട്ട് വർദ്ധിപ്പിക്കുന്നു. അളവ് ഇതിനകം അടച്ചുകൊള്ളാമെന്ന പോലും, 3-സ്റ്റാർ ബാഡ്ജുകൾ നേടാൻ പിന്നീട് തിരിച്ചെത്താം. ഒപ്പം, ഉയർന്ന സ്കോറുകൾ നേടാൻ എത്രയും വേഗം ഗെയിം പൂർത്തിയാക്കാൻ ശ്രമിക്കുക ആഗ്രഹിക്കുന്നു.
+മസ്തിഷ്ക-ബസിലും രസകരമായി സമാനതകളില്ലാത്തതായിരുന്നത് ഗെയിംപ്ലേ - മൃഗങ്ങൾ ഉരുട്ടി സഹായിക്കുന്നതിന് പരിസ്ഥിതി സംവദിക്കുക. ഗെയിം ഗൃഹാതുരന് എന്ന ബുദ്ധിമുട്ട് വർദ്ധിപ്പിക്കുന്നു. അളവ് ഇതിനകം അടച്ചുകൊള്ളാമെന്ന പോലും, 3-സ്റ്റാർ ബാഡ്ജുകൾ നേടാൻ പിന്നീട് തിരിച്ചെത്താം. ഒപ്പം, ഉയർന്ന സ്കോറുകൾ നേടാൻ എത്രയും വേഗം ഗെയിം പൂർത്തിയാക്കാൻ ശ്രമിക്കുക ആഗ്രഹിക്കുന്നു.
 പവർ യുപിഎസ് വെല്ലുവിളി തലങ്ങളിൽ കൈകാര്യം സഹായകരമായി.
 സുഖം ഗ്രാഫിക്സ് ആന്റ് സൌണ്ട് - ഗ്രാഫിക് വിശദാംശങ്ങൾ നന്നായി-സവാളും ശബ്ദങ്ങൾ മടിക്കേണ്ട. നാല് വ്യത്യസ്ത സാഹചര്യങ്ങളിലുള്ള ഉണ്ട് എല്ലാ രാപ്പകൽ പശ്ചാത്തലങ്ങൾ, കാലാവസ്ഥ ഇഫക്റ്റുകൾ, ആനിമേഷനുകൾ ടൺ അങ്ങനെ .സൂതികര്മ്മിണികള്. പ്രതീകങ്ങൾ '.അവരാരും സഹിക്കാനാവാത്ത ആണ്.
 കളിക്കുക ഗെയിം സേവനം ഉയർന്ന സ്കോറുകൾ സമർപ്പിക്കുന്നു കൂടുതൽ നേരമ്പോക്കിന് നേട്ടങ്ങളുടെ ടൺ അൺലോക്കാകുന്നു.
 ക്ലൗഡ് സംരക്ഷണം എളുപ്പത്തിൽ നിങ്ങളുടെ ഉപകരണങ്ങളിൽ തമ്മിലുള്ള ഗെയിം സമന്വയിപ്പിക്കപ്പെടുന്നു, ഇന്റർനെറ്റ് കണക്റ്റുചെയ്തിരിക്കുമ്പോഴാണ് പൂർണ്ണ ഗെയിം സവിശേഷതകൾ അൺലോക്കാകുന്നു.
 സുഹൃത്ത്, റാങ്കിംഗിൽ മാപ്പിൽ സുഹൃത്തുക്കൾ നോക്കിക്കൊണ്ടു നിങ്ങളുടെ മികച്ച ഫലങ്ങൾ പങ്കിടുന്നു, സുഹൃത്തുക്കളും നിന്നുള്ള സഹായവും അഭ്യർത്ഥിക്കുന്നു സ്കോർ, അയയ്ക്കുന്നതും ജീവിതത്തിൽ ആവശ്യപ്പെട്ട് കൂടുതൽ രസകരമായി സുഹൃത്തുക്കളുമായി പ്ലേ.
 സാർവത്രിക - വിവിധ ഗ്രാഫിക്സ് നിങ്ങളുടെ എല്ലാ ഉപകരണങ്ങളിലും fit സജ്ജമാക്കി. നിങ്ങളുടെ ഫോണുകളിലും ടാബ്ലറ്റുകളിലും ചടുലം പ്രതീകങ്ങൾ ആസ്വദിക്കുക.
-ചുരുൾ ഇതിനകം ഒരു ഫാൻ ഭക്ഷിച്ചില്ല?
+BannySammy ഇതിനകം ഒരു ഫാൻ?
 - Http://www.senspark.com ൽ ഞങ്ങളുടെ ഔദ്യോഗിക സൈറ്റ് സന്ദർശിക്കുക
 - Feedback@senspark.com വഴി നിങ്ങളുടെ ഫീഡ്ബാക്ക് അയയ്ക്കുക
-- തോന്നുന്നു &amp; https://www.facebook.com/TeamSenspark ഫോളോ</t>
+- തോന്നുന്നു &amp; https://www.facebook.com/TeamSenspark ഫോളോ
+*** അനുമതികൾ ***
+GET_ACCOUNTS: നിങ്ങൾ ലോഗിൻ അല്ലെങ്കിൽ Google + വഴി നിങ്ങളുടെ സുഹൃത്തുക്കളുമായി പ്ലേ അല്ലെങ്കിൽ പുഷ് അറിയിപ്പ് ലഭിക്കും ചെയ്യണമെങ്കിൽ മാത്രം ഉപയോഗിക്കുന്നു</t>
   </si>
   <si>
     <t>जंगल आमच्या गोंडस माकडे आणि अस्वल, सॅमी आणि Banny पदार्थांचे पूर्ण आहे. एक समस्या: अडथळे त्यांच्या आवडत्या हाताळते पोहोचत प्राणी प्रतिबंध. केळी आणि मध jars आणि अधिक त्यांना वाट शोधण्यासाठी प्रयत्न करा.
@@ -2045,10 +2159,12 @@
 मेघ जतन सहजपणे आपल्या डिव्हाइसेस दरम्यान खेळ समक्रमित करते आहे आणि त्याला इंटरनेटशी कनेक्ट केलेले असताना पूर्ण खेळ वैशिष्ट्ये उघडतो.
 मित्र मदत धावसंख्या पाठवणे आणि जीवन विचारत, मित्र, रँकिंग, नकाशावर मित्र पाहणे, आपल्या सर्वोत्तम परिणाम शेअर, आणि विनंती करून अधिक मजा मित्रांशी खेळू.
 युनिव्हर्सल - विविध ग्राफिक्स आपले डिव्हाइस सर्व फिट सेट केले जाते. आपल्या फोन आणि टॅबलेट खुसखुशीत वर्ण आनंद घ्या.
-आधीच नोंदीची आणि एक चाहता खा?
+आधीच BannySammy आवडला नाही?
 - Http://www.senspark.com आमच्या अधिकृत साइटला भेट द्या
 - Feedback@senspark.com द्वारे आपला अभिप्राय पाठवा
-- प्रमाणे आणि https://www.facebook.com/TeamSenspark वर अनुसरण</t>
+- प्रमाणे आणि https://www.facebook.com/TeamSenspark वर अनुसरण
+*** परवानग्या ***
+GET_ACCOUNTS: आपण लॉगिन करा किंवा Google + द्वारे आपल्या मित्रांशी खेळू किंवा पुश सूचना प्राप्त करू इच्छित असल्यास केवळ वापरले</t>
   </si>
   <si>
     <t>ширэнгэн ой нь бидний хөөрхөн сармагчин ба баавгай, Сэмми болон Banny нь хоол дүүрэн байдаг. Нэг асуудал нь: Бэрхшээл нь тэдний дуртай амттан хүрч мал урьдчилан сэргийлэх. Банан, зөгийн бал лонхтой, илүү тэднийг хүргэдэг замыг олохыг хичээ.
@@ -2056,17 +2172,19 @@
 амьтан тэдний хоол хүнс уруугаа тусал. Monkeys банана, алим, лийр болон идэж, баавгай яргай загас, зөгийн бал идэх. чулуун блок биш юм, харин Мод блок хэврэг байдаг. тоглоомын явцад дахь тоглолт зааврын ирэх илүү их тоглоом зүйлс байдаг.
 *** Тоглоомын онцлог ***
 Хавар, намар, өвөл, зуны: - 144 түвшинг 4 тохиолдолууд улиралд тус бүрт 36 түвшин байдаг. Хүн бүр өөр өөр тоглоом эд, улмаар сармагчин болон баавгай хооллож өөр стратеги байдаг.
-Тархи-Андреа зугаа нь өвөрмөц тоглоомын - мал уруугаа туслахын тулд байгаль орчны харилцах. тоглоомын явцад саад нэмэгдүүлдэг. Тэр ч байтугай түвшин аль хэдийн цэвэрлэж байгаа үед, та нар эргэж дараа нь 3 одтой тэмдэг олж ирж болно. Мөн, та хамгийн их оноо авахын тулд аль болох хурдан тоглолтыг дуусгаж хүсэж байна.
+Тархи-Андреа зугаа нь өвөрмөц тоглоомын - мал уруугаа туслах байгаль орчинд харилцах. тоглоомын явцад саад нэмэгдүүлдэг. Тэр ч байтугай түвшин аль хэдийн цэвэрлэж байгаа үед, та нар эргэж дараа нь 3 одтой тэмдэг олж ирж болно. Мөн, та хамгийн их оноо авахын тулд аль болох хурдан тоглолтыг дуусгаж хүсэж байна.
 POWER-UPS сорьсон түвшинд шийдвэрлэх нь тустай байдаг.
 Гайхалтай график болон SOUND - график дэлгэрэнгүй мэдээлэл, сайн холимог дуу мэдэр. дөрвөн өөр орчин байдаг, бүх өдөр, шөнө нь угсаа гарал, цаг агаарын нөлөө, мөн анимацыг тонн нь маш амьд байна. Зохиолын баатрууд, гол "cuteness тэвчихийн аргагүй юм.
 Тоглож тоглоомын үйлчилгээ өндөр оноо өргөн барьдаг, илүү хөгжилтэй нь амжилт тонн нээн илрүүлдэг.
 Cloud Save амархан захирах боломжоор хангадаг төхөөрөмжүүдийн хооронд тоглолтын синхрончлогдсон болон интернэтэд холбогдсон үед бүрэн тоглоомын боломжуудыг нээн илрүүлдэг.
 , Найз оноо, газрын зураг дээр найзуудаа харж, таны хамгийн сайн үр дүнг хуваалцах тусламж найз нөхөд нь илгээж, амь асууж тушаалын болон хүсэлт илүү хөгжилтэй нь найз нартайгаа хамт тоглоно.
 UNIVERSAL - Янз бүрийн график таны бүх төхөөрөмжүүдийг тохируулан тогтоосон байна. таны утас, таблет дээр яруу тэмдэгт сайхан өнгөрүүлээрэй.
-Аль хэдийн нэрийн болон сэнс идэх үү?
+Аль хэдийн BannySammy нь фен?
 - Http://www.senspark.com манай албан ёсны сайт руу орж авна уу
 - Feedback@senspark.com дамжуулан өөрийн санал хүсэлт илгээх
-- Like &amp; https://www.facebook.com/TeamSenspark дээр дагах</t>
+- Like &amp; https://www.facebook.com/TeamSenspark дээр дагах
+*** Зөвшөөрлүүд ***
+GET_ACCOUNTS: Зөвхөн танд нэвтрэх эсвэл Google + дамжуулан таны найз нөхөд хамт тоглох, эсвэл түлхэх мэдэгдэл хүлээн авах гэж байгаа бол ашиглаж</t>
   </si>
   <si>
     <t>यो जंगल हाम्रो प्यारा बाँदर र भालू, Sammy र Banny लागि खाद्य पदार्थ भरिएको छ। एक समस्या: अवरोध खडा आफ्नो मनपर्ने व्यवहार पुगन देखि जनावर रोक्न। केले र मह जार र थप तिनीहरूलाई जान्छ कि बाटो फेला पार्न प्रयास गर्नुहोस्।
@@ -2081,10 +2199,12 @@
 Cloud बचत सजिलै आफ्नो उपकरणहरू बीचको खेल सिंक र जब इन्टरनेटमा जडान पूर्ण खेल सुविधाहरू अनलक।
 साथीहरूबाट मद्दत स्कोर पठाउने र जीवन माग्दै, मित्र र्याङ्किङ्ग, नक्सामा मित्र हेर्दै, आफ्नो सबै भन्दा राम्रो परिणाम साझेदारी र अनुरोध गरेर थप रमाइलो संग साथीहरूसँग खेल्न।
 यूनिभर्सल - विभिन्न ग्राफिक्स आफ्नो सबै उपकरणहरु फिट सेट छन्। आफ्नो फोन र ट्याब्लेटमा कुरकुरा वर्ण आनन्द लिनुहोस्।
-पहिले नै रोल र एक प्रशंसक खानुहोस्?
+पहिले नै BannySammy को एक प्रशंसक?
 - Http://www.senspark.com हाम्रो आधिकारिक साइट भ्रमण
 - Feedback@senspark.com मार्फत आफ्नो प्रतिक्रिया पठाउनुहोस्
-- जस्तै र https://www.facebook.com/TeamSenspark मा पालन</t>
+- जस्तै र https://www.facebook.com/TeamSenspark मा पालन
+*** अनुमतिहरू ***
+GET_ACCOUNTS: तपाईं गर्नुहोस या गुगल + मार्फत आफ्नो साथीहरूसँग खेल्न वा पुस सूचना प्राप्त गर्न चाहनुहुन्छ भने मात्र प्रयोग</t>
   </si>
   <si>
     <t>جنگل پر از مواد غذایی برای میمون ناز ما و خرس، سمی و Banny است. یک مشکل: موانع جلوگیری از حیوانات را از رسیدن به رفتار مورد علاقه خود را. سعی کنید برای پیدا کردن مسیر که آنها را به موز و کوزه عسل و بیشتر منجر می شود.
@@ -2099,10 +2219,12 @@
 ابر ذخیره به راحتی بازی بین دستگاه های خود را همگام سازی و آنلاک ویژگی های کامل بازی به اینترنت متصل است.
 بازی با دوستان با لذت بیشتر با ارسال و درخواست برای زندگی، دوست نمره رتبه بندی، تماشای دوستان بر روی نقشه، به اشتراک گذاری بهترین نتایج خود را، و درخواست کمک از دوستان.
 UNIVERSAL - گرافیک های مختلف قرار است به همه جا از دستگاه های خود را. لذت بردن از شخصیت های ترد در گوشی ها و تبلت خود را.
-حال حاضر از طرفداران رول و خوردن؟
+حال حاضر از طرفداران BannySammy؟
 - سایت رسمی ما در http://www.senspark.com
 - ارسال بازخورد خود را از طریق feedback@senspark.com
-- مانند و به دنبال در https://www.facebook.com/TeamSenspark</t>
+- مانند و به دنبال در https://www.facebook.com/TeamSenspark
+*** مجوز ***
+GET_ACCOUNTS: تنها استفاده می شود اگر شما می خواهید برای ورود و یا بازی با دوستان خود از طریق گوگل + و یا دریافت هشدار از طریق فشار</t>
   </si>
   <si>
     <t>කැලේ අපගේ හුරුබුහුටි වඳුරු වලසුන්, සැමී හා Banny සඳහා ආහාර පිරී ඇත. එක් ගැටළුවක්: බාධක ඔවුන්ගේ ප්රියතම අමතා, ළඟාවීම සතුන් වැළැක්වීම. කෙසෙල් හා පැණි භාජන හා වැඩි කර ගැනීමට ඒවා මෙහෙය වන මාර්ගය සොයා ගැනීමට උත්සාහ කරන්න.
@@ -2117,10 +2239,12 @@
 Cloud SAVE පහසුවෙන් ඔබගේ උපාංග අතර ක්රීඩාව සමමුහුර්ත සහ අන්තර්ජාලය හා සම්බන්ධ වීමේදී සම්පූර්ණ ක්රීඩාව විශේෂාංග යතුරයි.
 මිතුරා පෙළේ, සිතියම මත මිතුරන් බලා, ඔබේ හොඳම ප්රතිඵල බෙදා, සහ මිතුරන් උදව් ඉල්ලා ලකුණු, යැවීම සහ ජීවිත අසමින් වැඩි විනෝදයක් සමග මිතුරන් සමග සෙල්ලම්.
 UNIVERSAL - විවිධ රූප ඔබගේ සියලු උපාංග ගැලපෙන ලෙස සකසා ඇත. ඔබගේ ජංගම දුරකථන හා ටැබ්ලට් මත කැඩෙන සුළු චරිත භුක්ති විඳින්න.
-Roll දැනටමත් රසිකයෙක් හා අනුභව?
+BannySammy දැනටමත් රසිකයෙක්?
 - Http://www.senspark.com අපගේ නිල වෙබ් අඩවිය වෙත පිවිසෙන්න
 - Feedback@senspark.com හරහා ඔබේ ප්රතිචාර
-- මෙන් සහ https://www.facebook.com/TeamSenspark මත අනුගමනය</t>
+- මෙන් සහ https://www.facebook.com/TeamSenspark මත අනුගමනය
+*** අවසර ***
+GET_ACCOUNTS: ඔබ ප්රවිෂ්ට වීම හෝ Google + හරහා ඔබේ මිතුරන් සමග සෙල්ලම් හෝ තල්ලුව නිවේදනයක් ලබා ගැනීමට අවශ්ය නම් පමණක් භාවිතා</t>
   </si>
   <si>
     <t>jungle ni kamili ya vyakula kwa nyani wetu cute na huzaa, Sammy na Banny. Tatizo moja: Vikwazo kuzuia wanyama kutoka kufikia chipsi yao favorite. Jaribu kupata njia ambayo inaongoza yao kwa ndizi na mitungi asali na zaidi.
@@ -2135,10 +2259,12 @@
 CLOUD SAVE urahisi syncs mchezo kati ya vifaa yako na unlocks makala mchezo full wakati wa kushikamana na Internet.
 Kucheza na marafiki na furaha zaidi kwa kutuma na kuuliza kwa maisha, rafiki alama cheo, kuangalia marafiki kwenye ramani, kugawana matokeo yako bora, na kuomba msaada kutoka kwa rafiki.
 UNIVERSAL - graphics mbalimbali ni kuweka na kifafa yote ya vifaa yako. Kufurahia wahusika crisp juu ya simu yako na vidonge.
-Tayari shabiki wa Unaendelea na kula?
+Tayari shabiki wa BannySammy?
 - Ziara tovuti yetu rasmi katika http://www.senspark.com
 - Tuma maoni yako kupitia feedback@senspark.com
-- Like &amp; kufuata juu https://www.facebook.com/TeamSenspark</t>
+- Like &amp; kufuata juu https://www.facebook.com/TeamSenspark
+*** Permissions ***
+GET_ACCOUNTS: kutumika Tu kama unataka kuingia katika au kucheza na rafiki yako kupitia Google + au kupokea kushinikiza taarifa</t>
   </si>
   <si>
     <t>காட்டில் எங்கள் அழகான குரங்குகள் மற்றும் கரடிகள், சம்மி மற்றும் Banny உணவுகள் முழு உள்ளது. ஒரு பிரச்சனை: தடைகளை தங்கள் பிடித்த விருந்தளித்து அடைவதில் இருந்து விலங்குகளை தடுக்க. வாழைப்பழங்கள் மற்றும் தேன் ஜாடிகளை மற்றும் இன்னும் அவர்களை இட்டு செல்கிறது என்று பாதை கண்டுபிடிக்க முயற்சி.
@@ -2153,10 +2279,12 @@
 மேகக்கணி சேமிப்பு எளிதாக உங்கள் சாதனங்கள் இடையே விளையாட்டு ஒத்திசைக்கிறது மற்றும் இணைய இணைப்பு போது முழு விளையாட்டு அம்சங்கள் திறக்கும்.
 நண்பர்கள் உதவி மதிப்பெண் நண்பர் அனுப்பும் மற்றும் உயிர்களை கேட்டு, தரவரிசை, வரைபடத்தில் நண்பர்கள் பார்த்து, உங்கள் சிறந்த முடிவுகளை பகிர்ந்து, மற்றும் கோரி இன்னும் வேடிக்கை உடன் நண்பர்களுடன் விளையாட.
 யுனிவர்சல் - வெவ்வேறு கிராபிக்ஸ் உங்கள் சாதனங்கள் அனைத்து பொருந்தும் அமைக்கப்பட்டுள்ளது. உங்கள் தொலைபேசிகள் மற்றும் மாத்திரைகள் மிருதுவான எழுத்துக்கள் உண்டு.
-ஏற்கனவே ரோல் மற்றும் ஒரு விசிறி சாப்பிட?
+ஏற்கனவே BannySammy ஒரு ரசிகர்?
 - Http://www.senspark.com எங்கள் அதிகாரப்பூர்வ தளத்திற்கு வருகை
 - Feedback@senspark.com வழியாக உங்கள் கருத்துக்களை அனுப்பவும்
-- போன்ற &amp; https://www.facebook.com/TeamSenspark பின்பற்ற</t>
+- போன்ற &amp; https://www.facebook.com/TeamSenspark பின்பற்ற
+*** அனுமதிகள் ***
+GET_ACCOUNTS: நீங்கள் உள்நுழைய அல்லது கூகுள் + வழியாக உங்கள் நண்பர்களுடன் விளையாட அல்லது புஷ் அறிவிப்பு பெற விரும்பினால் மட்டும் பயன்படுத்தப்படும்</t>
   </si>
   <si>
     <t>అడవి మా అందమైన కోతులు మరియు ఎలుగుబంట్లు, సమ్మీ మరియు Banny కోసం ఆహారాలు యొక్క నిండింది. ఒక సమస్య: అవరోధాలు వారి ఇష్టమైన కానుకల చేరకుండా జంతువులు నిరోధించడానికి. అరటి మరియు తేనె జాడి మరియు వాటిని మరో దారితీసే మార్గం కనుగొనేందుకు ప్రయత్నించండి.
@@ -2171,10 +2299,12 @@
 CLOUD రక్షించు సులభంగా మీ పరికరాల మధ్య ఆట సమకాలీకరిస్తుంది మరియు ఇంటర్నెట్ కనెక్ట్ చేసినప్పుడు పూర్తి ఆట లక్షణాలు అన్లాక్.
 స్నేహితుల నుండి సహాయం స్కోరు స్నేహితుడు పంపడం మరియు జీవితాలను కోరుతూ ర్యాంకింగ్కు, మాప్ లో స్నేహితులు చూడటం, మీ ఉత్తమ ఫలితాలు భాగస్వామ్యం, మరియు అభ్యర్థించడం ద్వారా మరింత సంతోషంతో స్నేహితులతో ప్లే.
 UNIVERSAL - వివిధ గ్రాఫిక్స్ మీ అన్ని పరికరాల్లో సరిపోయే కానున్నాయి. మీ ఫోన్లు మరియు టాబ్లెట్లలో స్ఫుటమైన అక్షరాలు ఆనందించండి.
-ఇప్పటికే రోల్ మరియు అభిమాని ఈట్?
+ఇప్పటికే BannySammy అభిమాని?
 - Http://www.senspark.com మా అధికారిక సైట్ సందర్శించండి
 - Feedback@senspark.com ద్వారా మీ అభిప్రాయాన్ని పంపండి
-- ఇలా &amp; https://www.facebook.com/TeamSenspark ఫాలో</t>
+- ఇలా &amp; https://www.facebook.com/TeamSenspark ఫాలో
+*** అనుమతులు ***
+GET_ACCOUNTS: మీరు లోనికి ప్రవేశించండి లేదా గూగుల్ + ద్వారా మీ స్నేహితులతో ప్లే లేదా పుష్ నోటిఫికేషన్ పొందాలనుకుంటున్నారా మాత్రమే ఉపయోగించాలి</t>
   </si>
   <si>
     <t>I hlathi ligcwele ukudla monkeys zethu cute namabhere, Sammy and Banny. Enye inkinga: Izithiyo ukuvimbela izilwane ingafiki awukudla abawuthandayo. Zama ukuthola indlela eholela ukuba ubhanana nezinyosi izimbiza ngaphezulu.
@@ -2189,10 +2319,12 @@
 Ukulondoloza kwefu Livumelanisa kalula umdlalo phakathi amadivayisi akho kanye ovula izici game full lapho uxhumeke kwi-Inthanethi.
 Ukudlala nabangani fun more ngokuthumela futhi ecela ukuphila, umngane score simo, ukubukela abangani ebalazweni, ukwabelana imiphumela yakho best, bacele usizo lwabangane.
 UNIVERSAL - Ihluzo Different ezibekwa ukuze uvumelane wonke amadivayisi akho. Jabulela izinhlamvu crisp amafoni akho kanye amaphilisi.
-Kakade fan of Roll kanye Yidla?
+Kakade a fan of BannySammy?
 - Vakashela ingosi yethu engokomthetho at http://www.senspark.com
 - Thumela impendulo yakho nge feedback@senspark.com
-- Like &amp; ukulandela https://www.facebook.com/TeamSenspark</t>
+- Like &amp; ukulandela https://www.facebook.com/TeamSenspark
+*** *** Izimvume
+Get_Accounts: esetshenziswa uma ufuna ungene ngemvume noma ukudlala nabangani bakho nge Google + noma ukwamukela push isaziso kuphela</t>
   </si>
   <si>
     <t>Youtube URL</t>
@@ -4716,7 +4848,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="7" ht="576.5" customHeight="1">
+    <row r="7" ht="644.35" customHeight="1">
       <c r="A7" t="s" s="3">
         <v>329</v>
       </c>

</xml_diff>